<commit_message>
superdataset-20 (without cons) test on mae
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-3.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-3.xlsx
@@ -381,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,8 +432,12 @@
       <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="J5" s="3">
+        <v>55.424267908505684</v>
+      </c>
+      <c r="K5" s="3">
+        <v>154.4179244249726</v>
+      </c>
     </row>
     <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
@@ -450,8 +454,12 @@
         <f>I5+1</f>
         <v>2</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="3">
+        <v>55.259116559375421</v>
+      </c>
+      <c r="K6" s="3">
+        <v>144.76450164293539</v>
+      </c>
     </row>
     <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
@@ -468,8 +476,12 @@
         <f t="shared" ref="I7:I54" si="1">I6+1</f>
         <v>3</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="3">
+        <v>55.017023695384189</v>
+      </c>
+      <c r="K7" s="3">
+        <v>154.58291894852141</v>
+      </c>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
@@ -486,8 +498,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="J8" s="3">
+        <v>55.424318586494998</v>
+      </c>
+      <c r="K8" s="3">
+        <v>145.71533953997809</v>
+      </c>
     </row>
     <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
@@ -504,8 +520,12 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="J9" s="3">
+        <v>56.229327489385021</v>
+      </c>
+      <c r="K9" s="3">
+        <v>143.66248630887179</v>
+      </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
@@ -522,8 +542,12 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="J10" s="3">
+        <v>55.303647445555399</v>
+      </c>
+      <c r="K10" s="3">
+        <v>146.41512595837901</v>
+      </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
@@ -540,8 +564,12 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="J11" s="3">
+        <v>55.923851527188063</v>
+      </c>
+      <c r="K11" s="3">
+        <v>142.85158269441399</v>
+      </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
@@ -558,8 +586,12 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="3">
+        <v>55.045093822764009</v>
+      </c>
+      <c r="K12" s="3">
+        <v>147.25348849945229</v>
+      </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
@@ -576,8 +608,12 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="J13" s="3">
+        <v>56.149997260649229</v>
+      </c>
+      <c r="K13" s="3">
+        <v>141.59311610076671</v>
+      </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
@@ -594,8 +630,12 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="3">
+        <v>55.989398712505128</v>
+      </c>
+      <c r="K14" s="3">
+        <v>141.10587075575029</v>
+      </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
@@ -612,8 +652,12 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="J15" s="3">
+        <v>54.829087796192297</v>
+      </c>
+      <c r="K15" s="3">
+        <v>150.3983515881709</v>
+      </c>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
@@ -630,8 +674,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="3">
+        <v>54.795221202574993</v>
+      </c>
+      <c r="K16" s="3">
+        <v>153.0842332968237</v>
+      </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
@@ -648,8 +696,12 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="J17" s="3">
+        <v>55.664584303520073</v>
+      </c>
+      <c r="K17" s="3">
+        <v>135.31889375684551</v>
+      </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
@@ -666,8 +718,12 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="J18" s="3">
+        <v>55.996336118339947</v>
+      </c>
+      <c r="K18" s="3">
+        <v>142.65653340635271</v>
+      </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
@@ -684,8 +740,12 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="J19" s="3">
+        <v>55.156718257772901</v>
+      </c>
+      <c r="K19" s="3">
+        <v>149.92729463307779</v>
+      </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
@@ -702,8 +762,12 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
+      <c r="J20" s="3">
+        <v>55.584656896315558</v>
+      </c>
+      <c r="K20" s="3">
+        <v>142.1763855421687</v>
+      </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
@@ -720,8 +784,12 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
+      <c r="J21" s="3">
+        <v>54.96366388166004</v>
+      </c>
+      <c r="K21" s="3">
+        <v>147.24496166484121</v>
+      </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
@@ -738,8 +806,12 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
+      <c r="J22" s="3">
+        <v>54.568407067524987</v>
+      </c>
+      <c r="K22" s="3">
+        <v>155.1026067907996</v>
+      </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
@@ -756,8 +828,12 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
+      <c r="J23" s="3">
+        <v>54.478741268319411</v>
+      </c>
+      <c r="K23" s="3">
+        <v>154.83286966046001</v>
+      </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
@@ -774,8 +850,12 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
+      <c r="J24" s="3">
+        <v>55.370594439117923</v>
+      </c>
+      <c r="K24" s="3">
+        <v>148.98651150054761</v>
+      </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
@@ -792,8 +872,12 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="J25" s="3">
+        <v>55.134302150390347</v>
+      </c>
+      <c r="K25" s="3">
+        <v>155.00518072289151</v>
+      </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
@@ -810,8 +894,12 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="3">
+        <v>55.907507190795783</v>
+      </c>
+      <c r="K26" s="3">
+        <v>131.24786418400879</v>
+      </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
@@ -828,8 +916,12 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="J27" s="3">
+        <v>55.533096836049857</v>
+      </c>
+      <c r="K27" s="3">
+        <v>146.29264512595839</v>
+      </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
@@ -846,8 +938,12 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
+      <c r="J28" s="3">
+        <v>55.050604026845633</v>
+      </c>
+      <c r="K28" s="3">
+        <v>147.51521358159911</v>
+      </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
@@ -864,8 +960,12 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="J29" s="3">
+        <v>54.789508286536091</v>
+      </c>
+      <c r="K29" s="3">
+        <v>153.77193318729459</v>
+      </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
@@ -882,8 +982,12 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
+      <c r="J30" s="3">
+        <v>54.549936994932203</v>
+      </c>
+      <c r="K30" s="3">
+        <v>148.3796166484118</v>
+      </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
@@ -900,8 +1004,12 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="J31" s="3">
+        <v>55.29320914943159</v>
+      </c>
+      <c r="K31" s="3">
+        <v>148.67573384446879</v>
+      </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
@@ -918,8 +1026,12 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
+      <c r="J32" s="3">
+        <v>55.050753321462807</v>
+      </c>
+      <c r="K32" s="3">
+        <v>146.82174151150051</v>
+      </c>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
@@ -936,8 +1048,12 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
+      <c r="J33" s="3">
+        <v>55.093511847692092</v>
+      </c>
+      <c r="K33" s="3">
+        <v>140.44404709748079</v>
+      </c>
     </row>
     <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
@@ -954,8 +1070,12 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
+      <c r="J34" s="3">
+        <v>54.987641418983713</v>
+      </c>
+      <c r="K34" s="3">
+        <v>152.9521029572837</v>
+      </c>
     </row>
     <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
@@ -972,8 +1092,12 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
+      <c r="J35" s="3">
+        <v>54.791792905081493</v>
+      </c>
+      <c r="K35" s="3">
+        <v>151.64943592552021</v>
+      </c>
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
@@ -990,8 +1114,12 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
+      <c r="J36" s="3">
+        <v>54.873843309135729</v>
+      </c>
+      <c r="K36" s="3">
+        <v>154.6143702081051</v>
+      </c>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
@@ -1008,8 +1136,12 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
+      <c r="J37" s="3">
+        <v>55.249631557320903</v>
+      </c>
+      <c r="K37" s="3">
+        <v>152.56055859802851</v>
+      </c>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
@@ -1026,8 +1158,12 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
+      <c r="J38" s="3">
+        <v>54.881038213943278</v>
+      </c>
+      <c r="K38" s="3">
+        <v>142.5526725082147</v>
+      </c>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
@@ -1044,8 +1180,12 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
+      <c r="J39" s="3">
+        <v>56.051006711409393</v>
+      </c>
+      <c r="K39" s="3">
+        <v>137.52119934282581</v>
+      </c>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
@@ -1062,8 +1202,12 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
+      <c r="J40" s="3">
+        <v>54.176366251198459</v>
+      </c>
+      <c r="K40" s="3">
+        <v>157.27287513691121</v>
+      </c>
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
@@ -1080,8 +1224,12 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
+      <c r="J41" s="3">
+        <v>53.988820709491847</v>
+      </c>
+      <c r="K41" s="3">
+        <v>163.01746440306681</v>
+      </c>
     </row>
     <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
@@ -1098,8 +1246,12 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
+      <c r="J42" s="3">
+        <v>56.263284481577863</v>
+      </c>
+      <c r="K42" s="3">
+        <v>142.6547864184009</v>
+      </c>
     </row>
     <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
@@ -1116,8 +1268,12 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
+      <c r="J43" s="3">
+        <v>56.314307629091907</v>
+      </c>
+      <c r="K43" s="3">
+        <v>138.63051478641839</v>
+      </c>
     </row>
     <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
@@ -1134,8 +1290,12 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
+      <c r="J44" s="3">
+        <v>56.142250376660719</v>
+      </c>
+      <c r="K44" s="3">
+        <v>139.37358159912381</v>
+      </c>
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
@@ -1152,8 +1312,12 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
+      <c r="J45" s="3">
+        <v>55.18708807012738</v>
+      </c>
+      <c r="K45" s="3">
+        <v>150.22291894852131</v>
+      </c>
     </row>
     <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
@@ -1170,8 +1334,12 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
+      <c r="J46" s="3">
+        <v>55.127571565538958</v>
+      </c>
+      <c r="K46" s="3">
+        <v>150.3330777656079</v>
+      </c>
     </row>
     <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
@@ -1188,8 +1356,12 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
+      <c r="J47" s="3">
+        <v>54.198056430625932</v>
+      </c>
+      <c r="K47" s="3">
+        <v>149.42481380065709</v>
+      </c>
     </row>
     <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
@@ -1206,8 +1378,12 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
+      <c r="J48" s="3">
+        <v>55.338035885495131</v>
+      </c>
+      <c r="K48" s="3">
+        <v>145.1532584884994</v>
+      </c>
     </row>
     <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
@@ -1224,8 +1400,12 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
+      <c r="J49" s="3">
+        <v>55.952420216408697</v>
+      </c>
+      <c r="K49" s="3">
+        <v>145.642004381161</v>
+      </c>
     </row>
     <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
@@ -1242,8 +1422,12 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
+      <c r="J50" s="3">
+        <v>55.455764963703608</v>
+      </c>
+      <c r="K50" s="3">
+        <v>145.42623767798469</v>
+      </c>
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
@@ -1260,8 +1444,12 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
+      <c r="J51" s="3">
+        <v>55.910698534447327</v>
+      </c>
+      <c r="K51" s="3">
+        <v>139.0867743702081</v>
+      </c>
     </row>
     <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
@@ -1278,8 +1466,12 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
+      <c r="J52" s="3">
+        <v>54.496575811532658</v>
+      </c>
+      <c r="K52" s="3">
+        <v>146.08871851040519</v>
+      </c>
     </row>
     <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
@@ -1296,8 +1488,12 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
+      <c r="J53" s="3">
+        <v>54.544969182303767</v>
+      </c>
+      <c r="K53" s="3">
+        <v>148.86469331872951</v>
+      </c>
     </row>
     <row r="54" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
@@ -1314,8 +1510,12 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
+      <c r="J54" s="3">
+        <v>55.698081084782899</v>
+      </c>
+      <c r="K54" s="3">
+        <v>142.90341182913471</v>
+      </c>
     </row>
     <row r="56" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
@@ -1332,13 +1532,13 @@
       <c r="I56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J56" s="3" t="e">
+      <c r="J56" s="3">
         <f>AVERAGE(J5:J54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K56" s="3" t="e">
+        <v>55.264114587042876</v>
+      </c>
+      <c r="K56" s="3">
         <f>AVERAGE(K5:K54)</f>
-        <v>#DIV/0!</v>
+        <v>147.12380887185103</v>
       </c>
     </row>
     <row r="57" spans="4:11" x14ac:dyDescent="0.25">
@@ -1356,13 +1556,13 @@
       <c r="I57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J57" s="3" t="e">
+      <c r="J57" s="3">
         <f>_xlfn.STDEV.S(J5:J54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K57" s="3" t="e">
+        <v>0.58747358219930423</v>
+      </c>
+      <c r="K57" s="3">
         <f>_xlfn.STDEV.S(K5:K54)</f>
-        <v>#DIV/0!</v>
+        <v>6.174332269252286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
superdataset-21 without cons test on mae
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-3.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-20.csv without cons)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-21.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-21.csv without cons)</t>
   </si>
 </sst>
 </file>
@@ -379,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:K57"/>
+  <dimension ref="D3:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,9 +397,13 @@
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
@@ -402,8 +412,16 @@
         <v>5</v>
       </c>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>0</v>
@@ -418,8 +436,22 @@
       <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N4" s="2"/>
+      <c r="O4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -438,8 +470,22 @@
       <c r="K5" s="3">
         <v>154.4179244249726</v>
       </c>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>53.738101629913707</v>
+      </c>
+      <c r="P5" s="3">
+        <v>149.63628696604599</v>
+      </c>
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+    </row>
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <f>D5+1</f>
         <v>2</v>
@@ -460,8 +506,24 @@
       <c r="K6" s="3">
         <v>144.76450164293539</v>
       </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N6" s="2">
+        <f>N5+1</f>
+        <v>2</v>
+      </c>
+      <c r="O6" s="3">
+        <v>53.541086152581833</v>
+      </c>
+      <c r="P6" s="3">
+        <v>155.15138554216861</v>
+      </c>
+      <c r="S6" s="2">
+        <f>S5+1</f>
+        <v>2</v>
+      </c>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+    </row>
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f t="shared" ref="D7:D54" si="0">D6+1</f>
         <v>3</v>
@@ -482,8 +544,24 @@
       <c r="K7" s="3">
         <v>154.58291894852141</v>
       </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N7" s="2">
+        <f t="shared" ref="N7:N54" si="2">N6+1</f>
+        <v>3</v>
+      </c>
+      <c r="O7" s="3">
+        <v>54.689241199835642</v>
+      </c>
+      <c r="P7" s="3">
+        <v>143.13598028477551</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" ref="S7:S54" si="3">S6+1</f>
+        <v>3</v>
+      </c>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+    </row>
+    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -504,8 +582,24 @@
       <c r="K8" s="3">
         <v>145.71533953997809</v>
       </c>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O8" s="3">
+        <v>55.263889878098887</v>
+      </c>
+      <c r="P8" s="3">
+        <v>147.5578587075575</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -526,8 +620,24 @@
       <c r="K9" s="3">
         <v>143.66248630887179</v>
       </c>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O9" s="3">
+        <v>54.32085330776605</v>
+      </c>
+      <c r="P9" s="3">
+        <v>150.0395071193866</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+    </row>
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -548,8 +658,24 @@
       <c r="K10" s="3">
         <v>146.41512595837901</v>
       </c>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O10" s="3">
+        <v>53.648561840843733</v>
+      </c>
+      <c r="P10" s="3">
+        <v>151.0301150054764</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+    </row>
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -570,8 +696,24 @@
       <c r="K11" s="3">
         <v>142.85158269441399</v>
       </c>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O11" s="3">
+        <v>55.223594028215309</v>
+      </c>
+      <c r="P11" s="3">
+        <v>144.29275465498361</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+    </row>
+    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -592,8 +734,24 @@
       <c r="K12" s="3">
         <v>147.25348849945229</v>
       </c>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O12" s="3">
+        <v>56.055545815641693</v>
+      </c>
+      <c r="P12" s="3">
+        <v>144.4272289156626</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+    </row>
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -614,8 +772,24 @@
       <c r="K13" s="3">
         <v>141.59311610076671</v>
       </c>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O13" s="3">
+        <v>54.098357759211062</v>
+      </c>
+      <c r="P13" s="3">
+        <v>148.92030668127049</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+    </row>
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -636,8 +810,24 @@
       <c r="K14" s="3">
         <v>141.10587075575029</v>
       </c>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O14" s="3">
+        <v>53.979420627311328</v>
+      </c>
+      <c r="P14" s="3">
+        <v>144.86430449068999</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+    </row>
+    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -658,8 +848,24 @@
       <c r="K15" s="3">
         <v>150.3983515881709</v>
       </c>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O15" s="3">
+        <v>54.930138337214082</v>
+      </c>
+      <c r="P15" s="3">
+        <v>144.82167579408539</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -680,8 +886,24 @@
       <c r="K16" s="3">
         <v>153.0842332968237</v>
       </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O16" s="3">
+        <v>54.679001506642933</v>
+      </c>
+      <c r="P16" s="3">
+        <v>149.10549288061341</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+    </row>
+    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -702,8 +924,24 @@
       <c r="K17" s="3">
         <v>135.31889375684551</v>
       </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O17" s="3">
+        <v>54.275036296397751</v>
+      </c>
+      <c r="P17" s="3">
+        <v>148.91654983570649</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+    </row>
+    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -724,8 +962,24 @@
       <c r="K18" s="3">
         <v>142.65653340635271</v>
       </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O18" s="3">
+        <v>55.587652376386792</v>
+      </c>
+      <c r="P18" s="3">
+        <v>137.2727875136911</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -746,8 +1000,24 @@
       <c r="K19" s="3">
         <v>149.92729463307779</v>
       </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O19" s="3">
+        <v>54.572720175318452</v>
+      </c>
+      <c r="P19" s="3">
+        <v>150.0026286966046</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+    </row>
+    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -768,8 +1038,24 @@
       <c r="K20" s="3">
         <v>142.1763855421687</v>
       </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O20" s="3">
+        <v>55.135577318175592</v>
+      </c>
+      <c r="P20" s="3">
+        <v>142.2148247535597</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+    </row>
+    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -790,8 +1076,24 @@
       <c r="K21" s="3">
         <v>147.24496166484121</v>
       </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O21" s="3">
+        <v>56.103305026708661</v>
+      </c>
+      <c r="P21" s="3">
+        <v>137.2438225629792</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+    </row>
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -812,8 +1114,24 @@
       <c r="K22" s="3">
         <v>155.1026067907996</v>
       </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O22" s="3">
+        <v>54.027246952472261</v>
+      </c>
+      <c r="P22" s="3">
+        <v>152.57814348302301</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -834,8 +1152,24 @@
       <c r="K23" s="3">
         <v>154.83286966046001</v>
       </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O23" s="3">
+        <v>54.471531297082599</v>
+      </c>
+      <c r="P23" s="3">
+        <v>144.17922234392111</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -856,8 +1190,24 @@
       <c r="K24" s="3">
         <v>148.98651150054761</v>
       </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O24" s="3">
+        <v>54.502900972469533</v>
+      </c>
+      <c r="P24" s="3">
+        <v>148.42997261774369</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+    </row>
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -878,8 +1228,24 @@
       <c r="K25" s="3">
         <v>155.00518072289151</v>
       </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O25" s="3">
+        <v>54.791131351869602</v>
+      </c>
+      <c r="P25" s="3">
+        <v>146.03740963855421</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+    </row>
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -900,8 +1266,24 @@
       <c r="K26" s="3">
         <v>131.24786418400879</v>
       </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O26" s="3">
+        <v>54.756736063552943</v>
+      </c>
+      <c r="P26" s="3">
+        <v>145.6442661555312</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+    </row>
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -922,8 +1304,24 @@
       <c r="K27" s="3">
         <v>146.29264512595839</v>
       </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O27" s="3">
+        <v>54.209411039583607</v>
+      </c>
+      <c r="P27" s="3">
+        <v>145.0289649507119</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+    </row>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -944,8 +1342,24 @@
       <c r="K28" s="3">
         <v>147.51521358159911</v>
       </c>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O28" s="3">
+        <v>55.295178742638001</v>
+      </c>
+      <c r="P28" s="3">
+        <v>136.14734939759029</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+    </row>
+    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -966,8 +1380,24 @@
       <c r="K29" s="3">
         <v>153.77193318729459</v>
       </c>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O29" s="3">
+        <v>54.224766470346523</v>
+      </c>
+      <c r="P29" s="3">
+        <v>151.0955969331873</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+    </row>
+    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -988,8 +1418,24 @@
       <c r="K30" s="3">
         <v>148.3796166484118</v>
       </c>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O30" s="3">
+        <v>54.310672510614992</v>
+      </c>
+      <c r="P30" s="3">
+        <v>141.89998904709751</v>
+      </c>
+      <c r="S30" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+    </row>
+    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1010,8 +1456,24 @@
       <c r="K31" s="3">
         <v>148.67573384446879</v>
       </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O31" s="3">
+        <v>53.767460621832619</v>
+      </c>
+      <c r="P31" s="3">
+        <v>152.50776560788611</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+    </row>
+    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1032,8 +1494,24 @@
       <c r="K32" s="3">
         <v>146.82174151150051</v>
       </c>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O32" s="3">
+        <v>54.553750171209423</v>
+      </c>
+      <c r="P32" s="3">
+        <v>141.51168674698789</v>
+      </c>
+      <c r="S32" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+    </row>
+    <row r="33" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1054,8 +1532,24 @@
       <c r="K33" s="3">
         <v>140.44404709748079</v>
       </c>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O33" s="3">
+        <v>54.719635666347081</v>
+      </c>
+      <c r="P33" s="3">
+        <v>141.1243318729463</v>
+      </c>
+      <c r="S33" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+    </row>
+    <row r="34" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1076,8 +1570,24 @@
       <c r="K34" s="3">
         <v>152.9521029572837</v>
       </c>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O34" s="3">
+        <v>54.396527872894133</v>
+      </c>
+      <c r="P34" s="3">
+        <v>141.574282584885</v>
+      </c>
+      <c r="S34" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+    </row>
+    <row r="35" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1098,8 +1608,24 @@
       <c r="K35" s="3">
         <v>151.64943592552021</v>
       </c>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O35" s="3">
+        <v>54.684310368442667</v>
+      </c>
+      <c r="P35" s="3">
+        <v>146.70938116100771</v>
+      </c>
+      <c r="S35" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+    </row>
+    <row r="36" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1120,8 +1646,24 @@
       <c r="K36" s="3">
         <v>154.6143702081051</v>
       </c>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O36" s="3">
+        <v>53.890987535953983</v>
+      </c>
+      <c r="P36" s="3">
+        <v>142.65382803943041</v>
+      </c>
+      <c r="S36" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+    </row>
+    <row r="37" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1142,8 +1684,24 @@
       <c r="K37" s="3">
         <v>152.56055859802851</v>
       </c>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O37" s="3">
+        <v>54.056327900287627</v>
+      </c>
+      <c r="P37" s="3">
+        <v>146.14921686746979</v>
+      </c>
+      <c r="S37" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+    </row>
+    <row r="38" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1164,8 +1722,24 @@
       <c r="K38" s="3">
         <v>142.5526725082147</v>
       </c>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O38" s="3">
+        <v>54.379254896589508</v>
+      </c>
+      <c r="P38" s="3">
+        <v>149.293587075575</v>
+      </c>
+      <c r="S38" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+    </row>
+    <row r="39" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1186,8 +1760,24 @@
       <c r="K39" s="3">
         <v>137.52119934282581</v>
       </c>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O39" s="3">
+        <v>54.591487467470209</v>
+      </c>
+      <c r="P39" s="3">
+        <v>143.4984501642935</v>
+      </c>
+      <c r="S39" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+    </row>
+    <row r="40" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1208,8 +1798,24 @@
       <c r="K40" s="3">
         <v>157.27287513691121</v>
       </c>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O40" s="3">
+        <v>54.169628817970143</v>
+      </c>
+      <c r="P40" s="3">
+        <v>149.89188389923331</v>
+      </c>
+      <c r="S40" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+    </row>
+    <row r="41" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1230,8 +1836,24 @@
       <c r="K41" s="3">
         <v>163.01746440306681</v>
       </c>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O41" s="3">
+        <v>55.281335433502257</v>
+      </c>
+      <c r="P41" s="3">
+        <v>140.73727272727271</v>
+      </c>
+      <c r="S41" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+    </row>
+    <row r="42" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1252,8 +1874,24 @@
       <c r="K42" s="3">
         <v>142.6547864184009</v>
       </c>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O42" s="3">
+        <v>54.485656759348032</v>
+      </c>
+      <c r="P42" s="3">
+        <v>146.27437568455639</v>
+      </c>
+      <c r="S42" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+    </row>
+    <row r="43" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1274,8 +1912,24 @@
       <c r="K43" s="3">
         <v>138.63051478641839</v>
       </c>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O43" s="3">
+        <v>54.15623613203671</v>
+      </c>
+      <c r="P43" s="3">
+        <v>150.5310952902519</v>
+      </c>
+      <c r="S43" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+    </row>
+    <row r="44" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1296,8 +1950,24 @@
       <c r="K44" s="3">
         <v>139.37358159912381</v>
       </c>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O44" s="3">
+        <v>53.809669908231747</v>
+      </c>
+      <c r="P44" s="3">
+        <v>143.680443592552</v>
+      </c>
+      <c r="S44" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+    </row>
+    <row r="45" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1318,8 +1988,24 @@
       <c r="K45" s="3">
         <v>150.22291894852131</v>
       </c>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O45" s="3">
+        <v>53.297362005204761</v>
+      </c>
+      <c r="P45" s="3">
+        <v>150.5702683461117</v>
+      </c>
+      <c r="S45" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="T45" s="3"/>
+      <c r="U45" s="3"/>
+    </row>
+    <row r="46" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1340,8 +2026,24 @@
       <c r="K46" s="3">
         <v>150.3330777656079</v>
       </c>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O46" s="3">
+        <v>55.409305574578823</v>
+      </c>
+      <c r="P46" s="3">
+        <v>139.9791018619934</v>
+      </c>
+      <c r="S46" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+    </row>
+    <row r="47" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1362,8 +2064,24 @@
       <c r="K47" s="3">
         <v>149.42481380065709</v>
       </c>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O47" s="3">
+        <v>53.933847418161882</v>
+      </c>
+      <c r="P47" s="3">
+        <v>144.6483625410734</v>
+      </c>
+      <c r="S47" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+    </row>
+    <row r="48" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1384,8 +2102,24 @@
       <c r="K48" s="3">
         <v>145.1532584884994</v>
       </c>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O48" s="3">
+        <v>53.936604574715787</v>
+      </c>
+      <c r="P48" s="3">
+        <v>149.1498138006572</v>
+      </c>
+      <c r="S48" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+    </row>
+    <row r="49" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1406,8 +2140,24 @@
       <c r="K49" s="3">
         <v>145.642004381161</v>
       </c>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O49" s="3">
+        <v>53.876227913984387</v>
+      </c>
+      <c r="P49" s="3">
+        <v>154.67331872946329</v>
+      </c>
+      <c r="S49" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+    </row>
+    <row r="50" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1428,8 +2178,24 @@
       <c r="K50" s="3">
         <v>145.42623767798469</v>
       </c>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O50" s="3">
+        <v>54.473872072318862</v>
+      </c>
+      <c r="P50" s="3">
+        <v>146.68242059145669</v>
+      </c>
+      <c r="S50" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
+    </row>
+    <row r="51" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1450,8 +2216,24 @@
       <c r="K51" s="3">
         <v>139.0867743702081</v>
       </c>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O51" s="3">
+        <v>56.163641966853866</v>
+      </c>
+      <c r="P51" s="3">
+        <v>130.6130887185104</v>
+      </c>
+      <c r="S51" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+    </row>
+    <row r="52" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1472,8 +2254,24 @@
       <c r="K52" s="3">
         <v>146.08871851040519</v>
       </c>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O52" s="3">
+        <v>55.11714011779209</v>
+      </c>
+      <c r="P52" s="3">
+        <v>143.91588170865279</v>
+      </c>
+      <c r="S52" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+    </row>
+    <row r="53" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1494,8 +2292,24 @@
       <c r="K53" s="3">
         <v>148.86469331872951</v>
       </c>
-    </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O53" s="3">
+        <v>54.78606629228873</v>
+      </c>
+      <c r="P53" s="3">
+        <v>142.34866922234389</v>
+      </c>
+      <c r="S53" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+    </row>
+    <row r="54" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1516,8 +2330,24 @@
       <c r="K54" s="3">
         <v>142.90341182913471</v>
       </c>
-    </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O54" s="3">
+        <v>55.61784687029175</v>
+      </c>
+      <c r="P54" s="3">
+        <v>144.2873384446878</v>
+      </c>
+      <c r="S54" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="T54" s="3"/>
+      <c r="U54" s="3"/>
+    </row>
+    <row r="56" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1540,8 +2370,30 @@
         <f>AVERAGE(K5:K54)</f>
         <v>147.12380887185103</v>
       </c>
-    </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O56" s="3">
+        <f>AVERAGE(O5:O54)</f>
+        <v>54.559716860704015</v>
+      </c>
+      <c r="P56" s="3">
+        <f>AVERAGE(P5:P54)</f>
+        <v>145.65360580503827</v>
+      </c>
+      <c r="S56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T56" s="3" t="e">
+        <f>AVERAGE(T5:T54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U56" s="3" t="e">
+        <f>AVERAGE(U5:U54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>3</v>
       </c>
@@ -1563,6 +2415,28 @@
       <c r="K57" s="3">
         <f>_xlfn.STDEV.S(K5:K54)</f>
         <v>6.174332269252286</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O57" s="3">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
+        <v>0.67045652390581412</v>
+      </c>
+      <c r="P57" s="3">
+        <f>_xlfn.STDEV.S(P5:P54)</f>
+        <v>4.8655786075045011</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T57" s="3" t="e">
+        <f>_xlfn.STDEV.S(T5:T54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U57" s="3" t="e">
+        <f>_xlfn.STDEV.S(U5:U54)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
superdataset-21 (with cons) test on mae
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-3.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-3.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MAE" sheetId="1" r:id="rId1"/>
+    <sheet name="MSE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -43,6 +44,12 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-21.csv without cons)</t>
+  </si>
+  <si>
+    <t>train (MSE)</t>
+  </si>
+  <si>
+    <t>test (MSE)</t>
   </si>
 </sst>
 </file>
@@ -96,13 +103,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -385,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:U57"/>
+  <dimension ref="D3:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,7 +413,7 @@
     <col min="21" max="21" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
@@ -413,15 +423,15 @@
       </c>
       <c r="K3" s="1"/>
       <c r="N3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="R3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="S3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U3" s="1"/>
-    </row>
-    <row r="4" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>0</v>
@@ -443,15 +453,15 @@
       <c r="P4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="T4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -474,18 +484,22 @@
         <v>1</v>
       </c>
       <c r="O5" s="3">
+        <v>53.784685659498699</v>
+      </c>
+      <c r="P5" s="3">
+        <v>143.91414567360351</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+      <c r="S5" s="3">
         <v>53.738101629913707</v>
       </c>
-      <c r="P5" s="3">
+      <c r="T5" s="3">
         <v>149.63628696604599</v>
       </c>
-      <c r="S5" s="2">
-        <v>1</v>
-      </c>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-    </row>
-    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <f>D5+1</f>
         <v>2</v>
@@ -511,19 +525,23 @@
         <v>2</v>
       </c>
       <c r="O6" s="3">
+        <v>53.214029584988353</v>
+      </c>
+      <c r="P6" s="3">
+        <v>154.10534501642931</v>
+      </c>
+      <c r="R6" s="2">
+        <f>R5+1</f>
+        <v>2</v>
+      </c>
+      <c r="S6" s="3">
         <v>53.541086152581833</v>
       </c>
-      <c r="P6" s="3">
+      <c r="T6" s="3">
         <v>155.15138554216861</v>
       </c>
-      <c r="S6" s="2">
-        <f>S5+1</f>
-        <v>2</v>
-      </c>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-    </row>
-    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f t="shared" ref="D7:D54" si="0">D6+1</f>
         <v>3</v>
@@ -549,19 +567,23 @@
         <v>3</v>
       </c>
       <c r="O7" s="3">
+        <v>54.262453088618003</v>
+      </c>
+      <c r="P7" s="3">
+        <v>138.29381708652789</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" ref="R7:R54" si="3">R6+1</f>
+        <v>3</v>
+      </c>
+      <c r="S7" s="3">
         <v>54.689241199835642</v>
       </c>
-      <c r="P7" s="3">
+      <c r="T7" s="3">
         <v>143.13598028477551</v>
       </c>
-      <c r="S7" s="2">
-        <f t="shared" ref="S7:S54" si="3">S6+1</f>
-        <v>3</v>
-      </c>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-    </row>
-    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -587,19 +609,23 @@
         <v>4</v>
       </c>
       <c r="O8" s="3">
+        <v>53.289001506642933</v>
+      </c>
+      <c r="P8" s="3">
+        <v>146.98502190580501</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S8" s="3">
         <v>55.263889878098887</v>
       </c>
-      <c r="P8" s="3">
+      <c r="T8" s="3">
         <v>147.5578587075575</v>
       </c>
-      <c r="S8" s="2">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-    </row>
-    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -625,19 +651,23 @@
         <v>5</v>
       </c>
       <c r="O9" s="3">
+        <v>53.593400903985753</v>
+      </c>
+      <c r="P9" s="3">
+        <v>144.0552190580504</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S9" s="3">
         <v>54.32085330776605</v>
       </c>
-      <c r="P9" s="3">
+      <c r="T9" s="3">
         <v>150.0395071193866</v>
       </c>
-      <c r="S9" s="2">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-    </row>
-    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -663,19 +693,23 @@
         <v>6</v>
       </c>
       <c r="O10" s="3">
+        <v>54.472598274209012</v>
+      </c>
+      <c r="P10" s="3">
+        <v>138.94664293537789</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="S10" s="3">
         <v>53.648561840843733</v>
       </c>
-      <c r="P10" s="3">
+      <c r="T10" s="3">
         <v>151.0301150054764</v>
       </c>
-      <c r="S10" s="2">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-    </row>
-    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -701,19 +735,23 @@
         <v>7</v>
       </c>
       <c r="O11" s="3">
+        <v>54.48869059033008</v>
+      </c>
+      <c r="P11" s="3">
+        <v>143.2578203723987</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S11" s="3">
         <v>55.223594028215309</v>
       </c>
-      <c r="P11" s="3">
+      <c r="T11" s="3">
         <v>144.29275465498361</v>
       </c>
-      <c r="S11" s="2">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-    </row>
-    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -739,19 +777,23 @@
         <v>8</v>
       </c>
       <c r="O12" s="3">
+        <v>54.534502122996848</v>
+      </c>
+      <c r="P12" s="3">
+        <v>140.22982475355971</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="S12" s="3">
         <v>56.055545815641693</v>
       </c>
-      <c r="P12" s="3">
+      <c r="T12" s="3">
         <v>144.4272289156626</v>
       </c>
-      <c r="S12" s="2">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-    </row>
-    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -777,19 +819,23 @@
         <v>9</v>
       </c>
       <c r="O13" s="3">
+        <v>54.123966579920562</v>
+      </c>
+      <c r="P13" s="3">
+        <v>147.71330230010949</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="S13" s="3">
         <v>54.098357759211062</v>
       </c>
-      <c r="P13" s="3">
+      <c r="T13" s="3">
         <v>148.92030668127049</v>
       </c>
-      <c r="S13" s="2">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-    </row>
-    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -815,19 +861,23 @@
         <v>10</v>
       </c>
       <c r="O14" s="3">
+        <v>53.873667990686208</v>
+      </c>
+      <c r="P14" s="3">
+        <v>143.82629791894851</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="S14" s="3">
         <v>53.979420627311328</v>
       </c>
-      <c r="P14" s="3">
+      <c r="T14" s="3">
         <v>144.86430449068999</v>
       </c>
-      <c r="S14" s="2">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-    </row>
-    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -853,19 +903,23 @@
         <v>11</v>
       </c>
       <c r="O15" s="3">
+        <v>54.614218600191748</v>
+      </c>
+      <c r="P15" s="3">
+        <v>140.52619934282581</v>
+      </c>
+      <c r="R15" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="S15" s="3">
         <v>54.930138337214082</v>
       </c>
-      <c r="P15" s="3">
+      <c r="T15" s="3">
         <v>144.82167579408539</v>
       </c>
-      <c r="S15" s="2">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-    </row>
-    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -891,19 +945,23 @@
         <v>12</v>
       </c>
       <c r="O16" s="3">
+        <v>53.290488974113131</v>
+      </c>
+      <c r="P16" s="3">
+        <v>149.8963253012048</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="S16" s="3">
         <v>54.679001506642933</v>
       </c>
-      <c r="P16" s="3">
+      <c r="T16" s="3">
         <v>149.10549288061341</v>
       </c>
-      <c r="S16" s="2">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-    </row>
-    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -929,19 +987,23 @@
         <v>13</v>
       </c>
       <c r="O17" s="3">
+        <v>54.108828927544167</v>
+      </c>
+      <c r="P17" s="3">
+        <v>144.0732092004381</v>
+      </c>
+      <c r="R17" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="S17" s="3">
         <v>54.275036296397751</v>
       </c>
-      <c r="P17" s="3">
+      <c r="T17" s="3">
         <v>148.91654983570649</v>
       </c>
-      <c r="S17" s="2">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-    </row>
-    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -967,19 +1029,23 @@
         <v>14</v>
       </c>
       <c r="O18" s="3">
+        <v>53.474956855225308</v>
+      </c>
+      <c r="P18" s="3">
+        <v>142.85575027382251</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="S18" s="3">
         <v>55.587652376386792</v>
       </c>
-      <c r="P18" s="3">
+      <c r="T18" s="3">
         <v>137.2727875136911</v>
       </c>
-      <c r="S18" s="2">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-    </row>
-    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1005,19 +1071,23 @@
         <v>15</v>
       </c>
       <c r="O19" s="3">
+        <v>54.422175044514439</v>
+      </c>
+      <c r="P19" s="3">
+        <v>142.16788608981381</v>
+      </c>
+      <c r="R19" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="S19" s="3">
         <v>54.572720175318452</v>
       </c>
-      <c r="P19" s="3">
+      <c r="T19" s="3">
         <v>150.0026286966046</v>
       </c>
-      <c r="S19" s="2">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-    </row>
-    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1043,19 +1113,23 @@
         <v>16</v>
       </c>
       <c r="O20" s="3">
+        <v>52.864199424736327</v>
+      </c>
+      <c r="P20" s="3">
+        <v>150.49209200438111</v>
+      </c>
+      <c r="R20" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="S20" s="3">
         <v>55.135577318175592</v>
       </c>
-      <c r="P20" s="3">
+      <c r="T20" s="3">
         <v>142.2148247535597</v>
       </c>
-      <c r="S20" s="2">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-    </row>
-    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1081,19 +1155,23 @@
         <v>17</v>
       </c>
       <c r="O21" s="3">
+        <v>53.727731817559217</v>
+      </c>
+      <c r="P21" s="3">
+        <v>137.55433187294631</v>
+      </c>
+      <c r="R21" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="S21" s="3">
         <v>56.103305026708661</v>
       </c>
-      <c r="P21" s="3">
+      <c r="T21" s="3">
         <v>137.2438225629792</v>
       </c>
-      <c r="S21" s="2">
-        <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-    </row>
-    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1119,19 +1197,23 @@
         <v>18</v>
       </c>
       <c r="O22" s="3">
+        <v>53.7914888371456</v>
+      </c>
+      <c r="P22" s="3">
+        <v>148.88646768893761</v>
+      </c>
+      <c r="R22" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="S22" s="3">
         <v>54.027246952472261</v>
       </c>
-      <c r="P22" s="3">
+      <c r="T22" s="3">
         <v>152.57814348302301</v>
       </c>
-      <c r="S22" s="2">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-    </row>
-    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1157,19 +1239,23 @@
         <v>19</v>
       </c>
       <c r="O23" s="3">
+        <v>53.834899328859052</v>
+      </c>
+      <c r="P23" s="3">
+        <v>144.527891566265</v>
+      </c>
+      <c r="R23" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="S23" s="3">
         <v>54.471531297082599</v>
       </c>
-      <c r="P23" s="3">
+      <c r="T23" s="3">
         <v>144.17922234392111</v>
       </c>
-      <c r="S23" s="2">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-    </row>
-    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1195,19 +1281,23 @@
         <v>20</v>
       </c>
       <c r="O24" s="3">
+        <v>53.853637857827692</v>
+      </c>
+      <c r="P24" s="3">
+        <v>140.66682365826949</v>
+      </c>
+      <c r="R24" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="S24" s="3">
         <v>54.502900972469533</v>
       </c>
-      <c r="P24" s="3">
+      <c r="T24" s="3">
         <v>148.42997261774369</v>
       </c>
-      <c r="S24" s="2">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-    </row>
-    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1233,19 +1323,23 @@
         <v>21</v>
       </c>
       <c r="O25" s="3">
+        <v>54.690434187097658</v>
+      </c>
+      <c r="P25" s="3">
+        <v>143.57098028477549</v>
+      </c>
+      <c r="R25" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="S25" s="3">
         <v>54.791131351869602</v>
       </c>
-      <c r="P25" s="3">
+      <c r="T25" s="3">
         <v>146.03740963855421</v>
       </c>
-      <c r="S25" s="2">
-        <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-    </row>
-    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1271,19 +1365,23 @@
         <v>22</v>
       </c>
       <c r="O26" s="3">
+        <v>54.139080947815373</v>
+      </c>
+      <c r="P26" s="3">
+        <v>143.4827327491785</v>
+      </c>
+      <c r="R26" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="S26" s="3">
         <v>54.756736063552943</v>
       </c>
-      <c r="P26" s="3">
+      <c r="T26" s="3">
         <v>145.6442661555312</v>
       </c>
-      <c r="S26" s="2">
-        <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-    </row>
-    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1309,19 +1407,23 @@
         <v>23</v>
       </c>
       <c r="O27" s="3">
+        <v>54.256397753732372</v>
+      </c>
+      <c r="P27" s="3">
+        <v>145.32230010952901</v>
+      </c>
+      <c r="R27" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="S27" s="3">
         <v>54.209411039583607</v>
       </c>
-      <c r="P27" s="3">
+      <c r="T27" s="3">
         <v>145.0289649507119</v>
       </c>
-      <c r="S27" s="2">
-        <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-    </row>
-    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1347,19 +1449,23 @@
         <v>24</v>
       </c>
       <c r="O28" s="3">
+        <v>53.728349541158742</v>
+      </c>
+      <c r="P28" s="3">
+        <v>147.56652792990141</v>
+      </c>
+      <c r="R28" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="S28" s="3">
         <v>55.295178742638001</v>
       </c>
-      <c r="P28" s="3">
+      <c r="T28" s="3">
         <v>136.14734939759029</v>
       </c>
-      <c r="S28" s="2">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-    </row>
-    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1385,19 +1491,23 @@
         <v>25</v>
       </c>
       <c r="O29" s="3">
+        <v>52.99615943021503</v>
+      </c>
+      <c r="P29" s="3">
+        <v>151.2906736035049</v>
+      </c>
+      <c r="R29" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="S29" s="3">
         <v>54.224766470346523</v>
       </c>
-      <c r="P29" s="3">
+      <c r="T29" s="3">
         <v>151.0955969331873</v>
       </c>
-      <c r="S29" s="2">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-    </row>
-    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1423,19 +1533,23 @@
         <v>26</v>
       </c>
       <c r="O30" s="3">
+        <v>53.558107108615253</v>
+      </c>
+      <c r="P30" s="3">
+        <v>144.79804490690029</v>
+      </c>
+      <c r="R30" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="S30" s="3">
         <v>54.310672510614992</v>
       </c>
-      <c r="P30" s="3">
+      <c r="T30" s="3">
         <v>141.89998904709751</v>
       </c>
-      <c r="S30" s="2">
-        <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-    </row>
-    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1461,19 +1575,23 @@
         <v>27</v>
       </c>
       <c r="O31" s="3">
+        <v>53.407168880975213</v>
+      </c>
+      <c r="P31" s="3">
+        <v>145.53386637458931</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="S31" s="3">
         <v>53.767460621832619</v>
       </c>
-      <c r="P31" s="3">
+      <c r="T31" s="3">
         <v>152.50776560788611</v>
       </c>
-      <c r="S31" s="2">
-        <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-    </row>
-    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1499,19 +1617,23 @@
         <v>28</v>
       </c>
       <c r="O32" s="3">
+        <v>53.982425695110251</v>
+      </c>
+      <c r="P32" s="3">
+        <v>143.94797918948521</v>
+      </c>
+      <c r="R32" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="S32" s="3">
         <v>54.553750171209423</v>
       </c>
-      <c r="P32" s="3">
+      <c r="T32" s="3">
         <v>141.51168674698789</v>
       </c>
-      <c r="S32" s="2">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-    </row>
-    <row r="33" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1537,19 +1659,23 @@
         <v>29</v>
       </c>
       <c r="O33" s="3">
+        <v>53.723595397890698</v>
+      </c>
+      <c r="P33" s="3">
+        <v>150.1996659364732</v>
+      </c>
+      <c r="R33" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="S33" s="3">
         <v>54.719635666347081</v>
       </c>
-      <c r="P33" s="3">
+      <c r="T33" s="3">
         <v>141.1243318729463</v>
       </c>
-      <c r="S33" s="2">
-        <f t="shared" si="3"/>
-        <v>29</v>
-      </c>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-    </row>
-    <row r="34" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1575,19 +1701,23 @@
         <v>30</v>
       </c>
       <c r="O34" s="3">
+        <v>54.260672510614981</v>
+      </c>
+      <c r="P34" s="3">
+        <v>141.34740963855421</v>
+      </c>
+      <c r="R34" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="S34" s="3">
         <v>54.396527872894133</v>
       </c>
-      <c r="P34" s="3">
+      <c r="T34" s="3">
         <v>141.574282584885</v>
       </c>
-      <c r="S34" s="2">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-    </row>
-    <row r="35" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1613,19 +1743,23 @@
         <v>31</v>
       </c>
       <c r="O35" s="3">
+        <v>54.409602794137783</v>
+      </c>
+      <c r="P35" s="3">
+        <v>142.30330777656081</v>
+      </c>
+      <c r="R35" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="S35" s="3">
         <v>54.684310368442667</v>
       </c>
-      <c r="P35" s="3">
+      <c r="T35" s="3">
         <v>146.70938116100771</v>
       </c>
-      <c r="S35" s="2">
-        <f t="shared" si="3"/>
-        <v>31</v>
-      </c>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
-    </row>
-    <row r="36" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1651,19 +1785,23 @@
         <v>32</v>
       </c>
       <c r="O36" s="3">
+        <v>54.057285303383097</v>
+      </c>
+      <c r="P36" s="3">
+        <v>147.04030668127061</v>
+      </c>
+      <c r="R36" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="S36" s="3">
         <v>53.890987535953983</v>
       </c>
-      <c r="P36" s="3">
+      <c r="T36" s="3">
         <v>142.65382803943041</v>
       </c>
-      <c r="S36" s="2">
-        <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-    </row>
-    <row r="37" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1689,19 +1827,23 @@
         <v>33</v>
       </c>
       <c r="O37" s="3">
+        <v>54.648812491439529</v>
+      </c>
+      <c r="P37" s="3">
+        <v>144.0035432639649</v>
+      </c>
+      <c r="R37" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="S37" s="3">
         <v>54.056327900287627</v>
       </c>
-      <c r="P37" s="3">
+      <c r="T37" s="3">
         <v>146.14921686746979</v>
       </c>
-      <c r="S37" s="2">
-        <f t="shared" si="3"/>
-        <v>33</v>
-      </c>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
-    </row>
-    <row r="38" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1727,19 +1869,23 @@
         <v>34</v>
       </c>
       <c r="O38" s="3">
+        <v>53.01938364607588</v>
+      </c>
+      <c r="P38" s="3">
+        <v>157.50395947426071</v>
+      </c>
+      <c r="R38" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="S38" s="3">
         <v>54.379254896589508</v>
       </c>
-      <c r="P38" s="3">
+      <c r="T38" s="3">
         <v>149.293587075575</v>
       </c>
-      <c r="S38" s="2">
-        <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-    </row>
-    <row r="39" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1765,19 +1911,23 @@
         <v>35</v>
       </c>
       <c r="O39" s="3">
+        <v>54.619383646075867</v>
+      </c>
+      <c r="P39" s="3">
+        <v>138.7863745892661</v>
+      </c>
+      <c r="R39" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="S39" s="3">
         <v>54.591487467470209</v>
       </c>
-      <c r="P39" s="3">
+      <c r="T39" s="3">
         <v>143.4984501642935</v>
       </c>
-      <c r="S39" s="2">
-        <f t="shared" si="3"/>
-        <v>35</v>
-      </c>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-    </row>
-    <row r="40" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1803,19 +1953,23 @@
         <v>36</v>
       </c>
       <c r="O40" s="3">
+        <v>53.994285714285709</v>
+      </c>
+      <c r="P40" s="3">
+        <v>151.72590909090911</v>
+      </c>
+      <c r="R40" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="S40" s="3">
         <v>54.169628817970143</v>
       </c>
-      <c r="P40" s="3">
+      <c r="T40" s="3">
         <v>149.89188389923331</v>
       </c>
-      <c r="S40" s="2">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-    </row>
-    <row r="41" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1841,19 +1995,23 @@
         <v>37</v>
       </c>
       <c r="O41" s="3">
+        <v>54.301221750445137</v>
+      </c>
+      <c r="P41" s="3">
+        <v>145.2726779846659</v>
+      </c>
+      <c r="R41" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="S41" s="3">
         <v>55.281335433502257</v>
       </c>
-      <c r="P41" s="3">
+      <c r="T41" s="3">
         <v>140.73727272727271</v>
       </c>
-      <c r="S41" s="2">
-        <f t="shared" si="3"/>
-        <v>37</v>
-      </c>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-    </row>
-    <row r="42" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1879,19 +2037,23 @@
         <v>38</v>
       </c>
       <c r="O42" s="3">
+        <v>53.286273113272138</v>
+      </c>
+      <c r="P42" s="3">
+        <v>153.73702081051479</v>
+      </c>
+      <c r="R42" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="S42" s="3">
         <v>54.485656759348032</v>
       </c>
-      <c r="P42" s="3">
+      <c r="T42" s="3">
         <v>146.27437568455639</v>
       </c>
-      <c r="S42" s="2">
-        <f t="shared" si="3"/>
-        <v>38</v>
-      </c>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-    </row>
-    <row r="43" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1917,19 +2079,23 @@
         <v>39</v>
       </c>
       <c r="O43" s="3">
+        <v>53.891013559786337</v>
+      </c>
+      <c r="P43" s="3">
+        <v>141.17922234392111</v>
+      </c>
+      <c r="R43" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="S43" s="3">
         <v>54.15623613203671</v>
       </c>
-      <c r="P43" s="3">
+      <c r="T43" s="3">
         <v>150.5310952902519</v>
       </c>
-      <c r="S43" s="2">
-        <f t="shared" si="3"/>
-        <v>39</v>
-      </c>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
-    </row>
-    <row r="44" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1955,19 +2121,23 @@
         <v>40</v>
       </c>
       <c r="O44" s="3">
+        <v>54.607381180660177</v>
+      </c>
+      <c r="P44" s="3">
+        <v>133.10432092004379</v>
+      </c>
+      <c r="R44" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="S44" s="3">
         <v>53.809669908231747</v>
       </c>
-      <c r="P44" s="3">
+      <c r="T44" s="3">
         <v>143.680443592552</v>
       </c>
-      <c r="S44" s="2">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
-    </row>
-    <row r="45" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1993,19 +2163,23 @@
         <v>41</v>
       </c>
       <c r="O45" s="3">
+        <v>54.075454047390771</v>
+      </c>
+      <c r="P45" s="3">
+        <v>146.31917305585981</v>
+      </c>
+      <c r="R45" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="S45" s="3">
         <v>53.297362005204761</v>
       </c>
-      <c r="P45" s="3">
+      <c r="T45" s="3">
         <v>150.5702683461117</v>
       </c>
-      <c r="S45" s="2">
-        <f t="shared" si="3"/>
-        <v>41</v>
-      </c>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
-    </row>
-    <row r="46" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2031,19 +2205,23 @@
         <v>42</v>
       </c>
       <c r="O46" s="3">
+        <v>53.30212025749897</v>
+      </c>
+      <c r="P46" s="3">
+        <v>149.65907995618841</v>
+      </c>
+      <c r="R46" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="S46" s="3">
         <v>55.409305574578823</v>
       </c>
-      <c r="P46" s="3">
+      <c r="T46" s="3">
         <v>139.9791018619934</v>
       </c>
-      <c r="S46" s="2">
-        <f t="shared" si="3"/>
-        <v>42</v>
-      </c>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-    </row>
-    <row r="47" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2069,19 +2247,23 @@
         <v>43</v>
       </c>
       <c r="O47" s="3">
+        <v>54.085636214217232</v>
+      </c>
+      <c r="P47" s="3">
+        <v>148.54654983570649</v>
+      </c>
+      <c r="R47" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="S47" s="3">
         <v>53.933847418161882</v>
       </c>
-      <c r="P47" s="3">
+      <c r="T47" s="3">
         <v>144.6483625410734</v>
       </c>
-      <c r="S47" s="2">
-        <f t="shared" si="3"/>
-        <v>43</v>
-      </c>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
-    </row>
-    <row r="48" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2107,19 +2289,23 @@
         <v>44</v>
       </c>
       <c r="O48" s="3">
+        <v>54.349705519791797</v>
+      </c>
+      <c r="P48" s="3">
+        <v>145.09336801752471</v>
+      </c>
+      <c r="R48" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="S48" s="3">
         <v>53.936604574715787</v>
       </c>
-      <c r="P48" s="3">
+      <c r="T48" s="3">
         <v>149.1498138006572</v>
       </c>
-      <c r="S48" s="2">
-        <f t="shared" si="3"/>
-        <v>44</v>
-      </c>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
-    </row>
-    <row r="49" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2145,19 +2331,23 @@
         <v>45</v>
       </c>
       <c r="O49" s="3">
+        <v>53.954259690453362</v>
+      </c>
+      <c r="P49" s="3">
+        <v>148.02246440306681</v>
+      </c>
+      <c r="R49" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="S49" s="3">
         <v>53.876227913984387</v>
       </c>
-      <c r="P49" s="3">
+      <c r="T49" s="3">
         <v>154.67331872946329</v>
       </c>
-      <c r="S49" s="2">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
-    </row>
-    <row r="50" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2183,19 +2373,23 @@
         <v>46</v>
       </c>
       <c r="O50" s="3">
+        <v>53.630127379810979</v>
+      </c>
+      <c r="P50" s="3">
+        <v>145.86639101861991</v>
+      </c>
+      <c r="R50" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="S50" s="3">
         <v>54.473872072318862</v>
       </c>
-      <c r="P50" s="3">
+      <c r="T50" s="3">
         <v>146.68242059145669</v>
       </c>
-      <c r="S50" s="2">
-        <f t="shared" si="3"/>
-        <v>46</v>
-      </c>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
-    </row>
-    <row r="51" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2221,19 +2415,23 @@
         <v>47</v>
       </c>
       <c r="O51" s="3">
+        <v>54.047929050814957</v>
+      </c>
+      <c r="P51" s="3">
+        <v>145.00038882803941</v>
+      </c>
+      <c r="R51" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="S51" s="3">
         <v>56.163641966853866</v>
       </c>
-      <c r="P51" s="3">
+      <c r="T51" s="3">
         <v>130.6130887185104</v>
       </c>
-      <c r="S51" s="2">
-        <f t="shared" si="3"/>
-        <v>47</v>
-      </c>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-    </row>
-    <row r="52" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2259,19 +2457,23 @@
         <v>48</v>
       </c>
       <c r="O52" s="3">
+        <v>54.194854129571283</v>
+      </c>
+      <c r="P52" s="3">
+        <v>141.6532475355969</v>
+      </c>
+      <c r="R52" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="S52" s="3">
         <v>55.11714011779209</v>
       </c>
-      <c r="P52" s="3">
+      <c r="T52" s="3">
         <v>143.91588170865279</v>
       </c>
-      <c r="S52" s="2">
-        <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-    </row>
-    <row r="53" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2297,19 +2499,23 @@
         <v>49</v>
       </c>
       <c r="O53" s="3">
+        <v>53.136627859197368</v>
+      </c>
+      <c r="P53" s="3">
+        <v>147.69013691128151</v>
+      </c>
+      <c r="R53" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="S53" s="3">
         <v>54.78606629228873</v>
       </c>
-      <c r="P53" s="3">
+      <c r="T53" s="3">
         <v>142.34866922234389</v>
       </c>
-      <c r="S53" s="2">
-        <f t="shared" si="3"/>
-        <v>49</v>
-      </c>
-      <c r="T53" s="3"/>
-      <c r="U53" s="3"/>
-    </row>
-    <row r="54" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2335,19 +2541,23 @@
         <v>50</v>
       </c>
       <c r="O54" s="3">
+        <v>53.421729900013688</v>
+      </c>
+      <c r="P54" s="3">
+        <v>152.60370208105149</v>
+      </c>
+      <c r="R54" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="S54" s="3">
         <v>55.61784687029175</v>
       </c>
-      <c r="P54" s="3">
+      <c r="T54" s="3">
         <v>144.2873384446878</v>
       </c>
-      <c r="S54" s="2">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="T54" s="3"/>
-      <c r="U54" s="3"/>
-    </row>
-    <row r="56" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2375,25 +2585,25 @@
       </c>
       <c r="O56" s="3">
         <f>AVERAGE(O5:O54)</f>
-        <v>54.559716860704015</v>
+        <v>53.907902013422827</v>
       </c>
       <c r="P56" s="3">
         <f>AVERAGE(P5:P54)</f>
+        <v>145.30291478641846</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S56" s="3">
+        <f>AVERAGE(S5:S54)</f>
+        <v>54.559716860704015</v>
+      </c>
+      <c r="T56" s="3">
+        <f>AVERAGE(T5:T54)</f>
         <v>145.65360580503827</v>
       </c>
-      <c r="S56" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="T56" s="3" t="e">
-        <f>AVERAGE(T5:T54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U56" s="3" t="e">
-        <f>AVERAGE(U5:U54)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="57" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>3</v>
       </c>
@@ -2421,21 +2631,480 @@
       </c>
       <c r="O57" s="3">
         <f>_xlfn.STDEV.S(O5:O54)</f>
-        <v>0.67045652390581412</v>
+        <v>0.48856022140286459</v>
       </c>
       <c r="P57" s="3">
         <f>_xlfn.STDEV.S(P5:P54)</f>
+        <v>4.6890659083821511</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S57" s="3">
+        <f>_xlfn.STDEV.S(S5:S54)</f>
+        <v>0.67045652390581412</v>
+      </c>
+      <c r="T57" s="3">
+        <f>_xlfn.STDEV.S(T5:T54)</f>
         <v>4.8655786075045011</v>
       </c>
-      <c r="S57" s="2" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D3:F57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <f>D5+1</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <f t="shared" ref="D7:D54" si="0">D6+1</f>
         <v>3</v>
       </c>
-      <c r="T57" s="3" t="e">
-        <f>_xlfn.STDEV.S(T5:T54)</f>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" s="4" t="e">
+        <f>AVERAGE(E5:E54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U57" s="3" t="e">
-        <f>_xlfn.STDEV.S(U5:U54)</f>
+      <c r="F56" s="4" t="e">
+        <f>AVERAGE(F5:F54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="4" t="e">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F57" s="4" t="e">
+        <f>_xlfn.STDEV.S(F5:F54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
superdataset-20 (without cons) test on mse
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-3.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -2656,25 +2656,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:F57"/>
+  <dimension ref="D3:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -2682,429 +2688,957 @@
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="4">
+        <v>1.2446644894602849E-4</v>
+      </c>
+      <c r="F5" s="4">
+        <v>6.1796445250980961E-4</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <f>D5+1</f>
         <v>2</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="4">
+        <v>1.1684232182386179E-4</v>
+      </c>
+      <c r="F6" s="4">
+        <v>9.0555319806772424E-4</v>
+      </c>
+      <c r="I6" s="2">
+        <f>I5+1</f>
+        <v>2</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f t="shared" ref="D7:D54" si="0">D6+1</f>
         <v>3</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="4">
+        <v>1.3064811918610399E-4</v>
+      </c>
+      <c r="F7" s="4">
+        <v>6.1581285621312588E-4</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" ref="I7:I54" si="1">I6+1</f>
+        <v>3</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="4">
+        <v>1.2907266383490931E-4</v>
+      </c>
+      <c r="F8" s="4">
+        <v>8.2228677010219174E-4</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="4">
+        <v>1.196053616554614E-4</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.131388841680097E-3</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="4">
+        <v>1.150768396915385E-4</v>
+      </c>
+      <c r="F10" s="4">
+        <v>8.7877762403024379E-4</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="4">
+        <v>1.3179345133859961E-4</v>
+      </c>
+      <c r="F11" s="4">
+        <v>8.1214201809106225E-4</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="4">
+        <v>1.27837345502081E-4</v>
+      </c>
+      <c r="F12" s="4">
+        <v>6.5823873704807818E-4</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="4">
+        <v>1.3510054044324821E-4</v>
+      </c>
+      <c r="F13" s="4">
+        <v>7.9729353656454911E-4</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="4">
+        <v>1.2781710482353241E-4</v>
+      </c>
+      <c r="F14" s="4">
+        <v>8.6198401991352677E-4</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="4">
+        <v>1.2443272577550871E-4</v>
+      </c>
+      <c r="F15" s="4">
+        <v>9.1678116028961565E-4</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="4">
+        <v>1.213836928698053E-4</v>
+      </c>
+      <c r="F16" s="4">
+        <v>7.4028997501118885E-4</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="4">
+        <v>1.331033592814548E-4</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7.1142868330732127E-4</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="4">
+        <v>1.2588106341208461E-4</v>
+      </c>
+      <c r="F18" s="4">
+        <v>9.6648374952556398E-4</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="4">
+        <v>1.314733622636012E-4</v>
+      </c>
+      <c r="F19" s="4">
+        <v>6.3127001127431099E-4</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="4">
+        <v>1.257135650161644E-4</v>
+      </c>
+      <c r="F20" s="4">
+        <v>8.4526032248125754E-4</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="4">
+        <v>1.2205393305489601E-4</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1.1109788447526961E-3</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="4">
+        <v>1.1028568841265881E-4</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1.1593087544397051E-3</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="4">
+        <v>1.2272213239451231E-4</v>
+      </c>
+      <c r="F23" s="4">
+        <v>6.4025357704196805E-4</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="4">
+        <v>1.3148820591888291E-4</v>
+      </c>
+      <c r="F24" s="4">
+        <v>6.9219512382108289E-4</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="4">
+        <v>1.172949587198428E-4</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1.011404424568403E-3</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="4">
+        <v>1.2448820086593781E-4</v>
+      </c>
+      <c r="F26" s="4">
+        <v>6.8853616420052764E-4</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="4">
+        <v>1.2257170547112881E-4</v>
+      </c>
+      <c r="F27" s="4">
+        <v>8.4712087769224498E-4</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="4">
+        <v>1.1912805621076321E-4</v>
+      </c>
+      <c r="F28" s="4">
+        <v>9.2631664213075119E-4</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="4">
+        <v>1.2707367681803329E-4</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1.052457409967145E-3</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="4">
+        <v>1.101209863337655E-4</v>
+      </c>
+      <c r="F30" s="4">
+        <v>1.066169818548743E-3</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E31" s="4">
+        <v>1.1631411971062931E-4</v>
+      </c>
+      <c r="F31" s="4">
+        <v>8.2252014019582834E-4</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="4">
+        <v>1.1691816707344799E-4</v>
+      </c>
+      <c r="F32" s="4">
+        <v>8.4187107257652205E-4</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="4">
+        <v>1.186602763214805E-4</v>
+      </c>
+      <c r="F33" s="4">
+        <v>8.439045204805169E-4</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="4">
+        <v>1.1581103370376969E-4</v>
+      </c>
+      <c r="F34" s="4">
+        <v>9.014769022625003E-4</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="4">
+        <v>1.165808712408225E-4</v>
+      </c>
+      <c r="F35" s="4">
+        <v>1.025380525361276E-3</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="4">
+        <v>1.149138524556614E-4</v>
+      </c>
+      <c r="F36" s="4">
+        <v>1.093108640349606E-3</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="4">
+        <v>1.161721732644664E-4</v>
+      </c>
+      <c r="F37" s="4">
+        <v>9.0313277977909076E-4</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="4">
+        <v>1.2013804201188541E-4</v>
+      </c>
+      <c r="F38" s="4">
+        <v>1.1092219520759631E-3</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="4">
+        <v>1.093439754658021E-4</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1.2470696650656221E-3</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="4">
+        <v>1.3200713218473401E-4</v>
+      </c>
+      <c r="F40" s="4">
+        <v>6.0641842384086134E-4</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E41" s="4">
+        <v>1.243893078757672E-4</v>
+      </c>
+      <c r="F41" s="4">
+        <v>6.4137284660238365E-4</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-    </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E42" s="4">
+        <v>1.2796915013832901E-4</v>
+      </c>
+      <c r="F42" s="4">
+        <v>7.842184876207509E-4</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-    </row>
-    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E43" s="4">
+        <v>1.26623201515188E-4</v>
+      </c>
+      <c r="F43" s="4">
+        <v>8.4674089676561458E-4</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-    </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E44" s="4">
+        <v>1.14893492568111E-4</v>
+      </c>
+      <c r="F44" s="4">
+        <v>1.1309888794191561E-3</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E45" s="4">
+        <v>1.2503425381630269E-4</v>
+      </c>
+      <c r="F45" s="4">
+        <v>8.1257762125139742E-4</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-    </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E46" s="4">
+        <v>1.0294523615547651E-4</v>
+      </c>
+      <c r="F46" s="4">
+        <v>1.46714595666021E-3</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E47" s="4">
+        <v>1.168407577686567E-4</v>
+      </c>
+      <c r="F47" s="4">
+        <v>8.7897910071153417E-4</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-    </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E48" s="4">
+        <v>1.221622187447097E-4</v>
+      </c>
+      <c r="F48" s="4">
+        <v>9.8622951537373168E-4</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-    </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E49" s="4">
+        <v>1.187631280360972E-4</v>
+      </c>
+      <c r="F49" s="4">
+        <v>1.057709492025047E-3</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-    </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E50" s="4">
+        <v>1.312275112482064E-4</v>
+      </c>
+      <c r="F50" s="4">
+        <v>8.4211498440781734E-4</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E51" s="4">
+        <v>1.2471372369474211E-4</v>
+      </c>
+      <c r="F51" s="4">
+        <v>7.4555923734151745E-4</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-    </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="4">
+        <v>1.113379617603689E-4</v>
+      </c>
+      <c r="F52" s="4">
+        <v>9.5659094739302373E-4</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-    </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E53" s="4">
+        <v>1.167654447349066E-4</v>
+      </c>
+      <c r="F53" s="4">
+        <v>9.5188505308882313E-4</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-    </row>
-    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E54" s="4">
+        <v>1.279191349390201E-4</v>
+      </c>
+      <c r="F54" s="4">
+        <v>8.439628751452543E-4</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="4" t="e">
+      <c r="E56" s="4">
         <f>AVERAGE(E5:E54)</f>
+        <v>1.2191839352985973E-4</v>
+      </c>
+      <c r="F56" s="4">
+        <f>AVERAGE(F5:F54)</f>
+        <v>8.8895756218133957E-4</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J56" s="4" t="e">
+        <f>AVERAGE(J5:J54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F56" s="4" t="e">
-        <f>AVERAGE(F5:F54)</f>
+      <c r="K56" s="4" t="e">
+        <f>AVERAGE(K5:K54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E57" s="4" t="e">
+      <c r="E57" s="4">
         <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>7.1459789974840207E-6</v>
+      </c>
+      <c r="F57" s="4">
+        <f>_xlfn.STDEV.S(F5:F54)</f>
+        <v>1.8171701498687141E-4</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J57" s="4" t="e">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F57" s="4" t="e">
-        <f>_xlfn.STDEV.S(F5:F54)</f>
+      <c r="K57" s="4" t="e">
+        <f>_xlfn.STDEV.S(K5:K54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
superdataset 20 (with cons) test on mse
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-3.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="10">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -2656,10 +2656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:K57"/>
+  <dimension ref="D3:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2668,19 +2668,25 @@
     <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -2695,8 +2701,15 @@
       <c r="K4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N4" s="2"/>
+      <c r="O4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -2709,10 +2722,19 @@
       <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="4">
+        <v>1.1509401918944859E-4</v>
+      </c>
+      <c r="K5" s="4">
+        <v>8.4596251713935642E-4</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <f>D5+1</f>
         <v>2</v>
@@ -2727,10 +2749,20 @@
         <f>I5+1</f>
         <v>2</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="4">
+        <v>1.0891381202107789E-4</v>
+      </c>
+      <c r="K6" s="4">
+        <v>7.7944262169602082E-4</v>
+      </c>
+      <c r="N6" s="2">
+        <f>N5+1</f>
+        <v>2</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f t="shared" ref="D7:D54" si="0">D6+1</f>
         <v>3</v>
@@ -2745,10 +2777,20 @@
         <f t="shared" ref="I7:I54" si="1">I6+1</f>
         <v>3</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="4">
+        <v>1.0154041121546049E-4</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1.068389897890192E-3</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" ref="N7:N54" si="2">N6+1</f>
+        <v>3</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2763,10 +2805,20 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="4">
+        <v>1.118512864312136E-4</v>
+      </c>
+      <c r="K8" s="4">
+        <v>9.3446588667570572E-4</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2781,10 +2833,20 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="4">
+        <v>1.1888193294917651E-4</v>
+      </c>
+      <c r="K9" s="4">
+        <v>7.1262290278773692E-4</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2799,10 +2861,20 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="4">
+        <v>1.103963584647762E-4</v>
+      </c>
+      <c r="K10" s="4">
+        <v>7.8850298554907611E-4</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+    </row>
+    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2817,10 +2889,20 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="4">
+        <v>1.170134769518971E-4</v>
+      </c>
+      <c r="K11" s="4">
+        <v>8.2365794256866374E-4</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+    </row>
+    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2835,10 +2917,20 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J12" s="4">
+        <v>1.1700085887599451E-4</v>
+      </c>
+      <c r="K12" s="4">
+        <v>8.1303807976297637E-4</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+    </row>
+    <row r="13" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2853,10 +2945,20 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="4">
+        <v>1.074416458598002E-4</v>
+      </c>
+      <c r="K13" s="4">
+        <v>8.6743831492659652E-4</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+    </row>
+    <row r="14" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2871,10 +2973,20 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="4">
+        <v>1.09577897553583E-4</v>
+      </c>
+      <c r="K14" s="4">
+        <v>7.0802050484675551E-4</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+    </row>
+    <row r="15" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2889,10 +3001,20 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="4">
+        <v>1.1146566473363199E-4</v>
+      </c>
+      <c r="K15" s="4">
+        <v>8.9522427310277511E-4</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2907,10 +3029,20 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="4">
+        <v>1.2881160144035639E-4</v>
+      </c>
+      <c r="K16" s="4">
+        <v>6.0547887566405408E-4</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2925,10 +3057,20 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="4">
+        <v>1.160116806879669E-4</v>
+      </c>
+      <c r="K17" s="4">
+        <v>7.8686201298070033E-4</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2943,10 +3085,20 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J18" s="4">
+        <v>1.151920989721826E-4</v>
+      </c>
+      <c r="K18" s="4">
+        <v>6.7529202615455408E-4</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+    </row>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2961,10 +3113,20 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="4">
+        <v>1.113182466093625E-4</v>
+      </c>
+      <c r="K19" s="4">
+        <v>6.4647392807658949E-4</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2979,10 +3141,20 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="4">
+        <v>1.0889015129475541E-4</v>
+      </c>
+      <c r="K20" s="4">
+        <v>8.0732353339916466E-4</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2997,10 +3169,20 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="4">
+        <v>1.101115699044487E-4</v>
+      </c>
+      <c r="K21" s="4">
+        <v>9.2270492758206736E-4</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+    </row>
+    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3015,10 +3197,20 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="4">
+        <v>1.043096559125857E-4</v>
+      </c>
+      <c r="K22" s="4">
+        <v>9.0528088851319038E-4</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+    </row>
+    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3033,10 +3225,20 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="4">
+        <v>1.194774964722091E-4</v>
+      </c>
+      <c r="K23" s="4">
+        <v>6.3690862694057492E-4</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+    </row>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3051,10 +3253,20 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="4">
+        <v>1.158794379207492E-4</v>
+      </c>
+      <c r="K24" s="4">
+        <v>6.6499789872208391E-4</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+    </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3069,10 +3281,20 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="4">
+        <v>1.2006704000425851E-4</v>
+      </c>
+      <c r="K25" s="4">
+        <v>8.2281318734743242E-4</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3087,10 +3309,20 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="4">
+        <v>1.115945781844151E-4</v>
+      </c>
+      <c r="K26" s="4">
+        <v>9.1529136256964373E-4</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+    </row>
+    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3105,10 +3337,20 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="4">
+        <v>1.129101404089035E-4</v>
+      </c>
+      <c r="K27" s="4">
+        <v>8.6871692800225757E-4</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+    </row>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3123,10 +3365,20 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J28" s="4">
+        <v>1.032695086839765E-4</v>
+      </c>
+      <c r="K28" s="4">
+        <v>9.3603048008748921E-4</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3141,10 +3393,20 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="4">
+        <v>1.146587046893823E-4</v>
+      </c>
+      <c r="K29" s="4">
+        <v>7.9716837329013134E-4</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3159,10 +3421,20 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J30" s="4">
+        <v>1.02154612558613E-4</v>
+      </c>
+      <c r="K30" s="4">
+        <v>1.3330071317397469E-3</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3177,10 +3449,20 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J31" s="4">
+        <v>1.12590788315525E-4</v>
+      </c>
+      <c r="K31" s="4">
+        <v>1.020304846375869E-3</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3195,10 +3477,20 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J32" s="4">
+        <v>1.0841652226814051E-4</v>
+      </c>
+      <c r="K32" s="4">
+        <v>7.8672498185434201E-4</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+    </row>
+    <row r="33" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3213,10 +3505,20 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J33" s="4">
+        <v>1.222480652536344E-4</v>
+      </c>
+      <c r="K33" s="4">
+        <v>6.1884673748703611E-4</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+    </row>
+    <row r="34" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3231,10 +3533,20 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J34" s="4">
+        <v>1.107273227631967E-4</v>
+      </c>
+      <c r="K34" s="4">
+        <v>7.7734611422439496E-4</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3249,10 +3561,20 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J35" s="4">
+        <v>1.178908565366489E-4</v>
+      </c>
+      <c r="K35" s="4">
+        <v>6.614372410414719E-4</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3267,10 +3589,20 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J36" s="4">
+        <v>1.061911727931064E-4</v>
+      </c>
+      <c r="K36" s="4">
+        <v>1.0836293647513259E-3</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+    </row>
+    <row r="37" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3285,10 +3617,20 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J37" s="4">
+        <v>1.158819714449737E-4</v>
+      </c>
+      <c r="K37" s="4">
+        <v>7.7567000667460467E-4</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+    </row>
+    <row r="38" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3303,10 +3645,20 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J38" s="4">
+        <v>1.214944951135354E-4</v>
+      </c>
+      <c r="K38" s="4">
+        <v>7.1180906644594747E-4</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+    </row>
+    <row r="39" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3321,10 +3673,20 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J39" s="4">
+        <v>1.100428270499541E-4</v>
+      </c>
+      <c r="K39" s="4">
+        <v>8.365367047279698E-4</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+    </row>
+    <row r="40" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3339,10 +3701,20 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J40" s="4">
+        <v>1.1740693895656139E-4</v>
+      </c>
+      <c r="K40" s="4">
+        <v>8.1723582250925149E-4</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+    </row>
+    <row r="41" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3357,10 +3729,20 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J41" s="4">
+        <v>1.14375185014424E-4</v>
+      </c>
+      <c r="K41" s="4">
+        <v>8.6023661076441865E-4</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+    </row>
+    <row r="42" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3375,10 +3757,20 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J42" s="4">
+        <v>1.159353146501999E-4</v>
+      </c>
+      <c r="K42" s="4">
+        <v>7.2700204670618019E-4</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+    </row>
+    <row r="43" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3393,10 +3785,20 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J43" s="4">
+        <v>1.111612736735101E-4</v>
+      </c>
+      <c r="K43" s="4">
+        <v>7.6137289673025479E-4</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+    </row>
+    <row r="44" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3411,10 +3813,20 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J44" s="4">
+        <v>1.198889625765995E-4</v>
+      </c>
+      <c r="K44" s="4">
+        <v>6.6171202802765741E-4</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+    </row>
+    <row r="45" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3429,10 +3841,20 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J45" s="4">
+        <v>1.104471776958471E-4</v>
+      </c>
+      <c r="K45" s="4">
+        <v>7.302408854739465E-4</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+    </row>
+    <row r="46" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3447,10 +3869,20 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J46" s="4">
+        <v>1.059238435859602E-4</v>
+      </c>
+      <c r="K46" s="4">
+        <v>9.7150380960080705E-4</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+    </row>
+    <row r="47" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3465,10 +3897,20 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J47" s="4">
+        <v>1.22426004213166E-4</v>
+      </c>
+      <c r="K47" s="4">
+        <v>8.1492842614850898E-4</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+    </row>
+    <row r="48" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3483,10 +3925,20 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J48" s="4">
+        <v>1.161235099756959E-4</v>
+      </c>
+      <c r="K48" s="4">
+        <v>7.0573380618306827E-4</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+    </row>
+    <row r="49" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3501,10 +3953,20 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J49" s="4">
+        <v>1.19698277375593E-4</v>
+      </c>
+      <c r="K49" s="4">
+        <v>7.3419598659927438E-4</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+    </row>
+    <row r="50" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3519,10 +3981,20 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J50" s="4">
+        <v>1.190421091684601E-4</v>
+      </c>
+      <c r="K50" s="4">
+        <v>6.5277229150685634E-4</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+    </row>
+    <row r="51" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3537,10 +4009,20 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J51" s="4">
+        <v>1.135124577623107E-4</v>
+      </c>
+      <c r="K51" s="4">
+        <v>1.007523653543452E-3</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+    </row>
+    <row r="52" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3555,10 +4037,20 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J52" s="4">
+        <v>1.113164752526531E-4</v>
+      </c>
+      <c r="K52" s="4">
+        <v>8.7143482313756335E-4</v>
+      </c>
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+    </row>
+    <row r="53" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3573,10 +4065,20 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-    </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J53" s="4">
+        <v>1.162135403229242E-4</v>
+      </c>
+      <c r="K53" s="4">
+        <v>6.5800478690999616E-4</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+    </row>
+    <row r="54" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3591,10 +4093,20 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-    </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J54" s="4">
+        <v>1.0465679180572701E-4</v>
+      </c>
+      <c r="K54" s="4">
+        <v>1.035666480828549E-3</v>
+      </c>
+      <c r="N54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+    </row>
+    <row r="56" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>2</v>
       </c>
@@ -3609,16 +4121,27 @@
       <c r="I56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J56" s="4" t="e">
+      <c r="J56" s="4">
         <f>AVERAGE(J5:J54)</f>
+        <v>1.1334891543117149E-4</v>
+      </c>
+      <c r="K56" s="4">
+        <f>AVERAGE(K5:K54)</f>
+        <v>8.1685971052536572E-4</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O56" s="4" t="e">
+        <f>AVERAGE(O5:O54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K56" s="4" t="e">
-        <f>AVERAGE(K5:K54)</f>
+      <c r="P56" s="4" t="e">
+        <f>AVERAGE(P5:P54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>3</v>
       </c>
@@ -3633,12 +4156,23 @@
       <c r="I57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J57" s="4" t="e">
+      <c r="J57" s="4">
         <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>5.7543411780092667E-6</v>
+      </c>
+      <c r="K57" s="4">
+        <f>_xlfn.STDEV.S(K5:K54)</f>
+        <v>1.4234407099589349E-4</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O57" s="4" t="e">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K57" s="4" t="e">
-        <f>_xlfn.STDEV.S(K5:K54)</f>
+      <c r="P57" s="4" t="e">
+        <f>_xlfn.STDEV.S(P5:P54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
superdataset-20 with cons test on mse
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-3.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -2656,10 +2656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:P57"/>
+  <dimension ref="D3:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2670,23 +2670,29 @@
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" customWidth="1"/>
+    <col min="20" max="20" width="15" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="S3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -2708,1472 +2714,2000 @@
       <c r="P4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="4">
-        <v>1.2446644894602849E-4</v>
+        <v>1.174206343922448E-4</v>
       </c>
       <c r="F5" s="4">
-        <v>6.1796445250980961E-4</v>
+        <v>7.603705663180799E-4</v>
       </c>
       <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="J5" s="4">
-        <v>1.1509401918944859E-4</v>
-      </c>
-      <c r="K5" s="4">
-        <v>8.4596251713935642E-4</v>
-      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
       <c r="N5" s="2">
         <v>1</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="O5" s="4">
+        <v>1.2446644894602849E-4</v>
+      </c>
+      <c r="P5" s="4">
+        <v>6.1796445250980961E-4</v>
+      </c>
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="T5" s="4">
+        <v>1.1509401918944859E-4</v>
+      </c>
+      <c r="U5" s="4">
+        <v>8.4596251713935642E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <f>D5+1</f>
         <v>2</v>
       </c>
       <c r="E6" s="4">
-        <v>1.1684232182386179E-4</v>
+        <v>1.140973705765286E-4</v>
       </c>
       <c r="F6" s="4">
-        <v>9.0555319806772424E-4</v>
+        <v>9.9928136189472E-4</v>
       </c>
       <c r="I6" s="2">
         <f>I5+1</f>
         <v>2</v>
       </c>
-      <c r="J6" s="4">
-        <v>1.0891381202107789E-4</v>
-      </c>
-      <c r="K6" s="4">
-        <v>7.7944262169602082E-4</v>
-      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
       <c r="N6" s="2">
         <f>N5+1</f>
         <v>2</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="O6" s="4">
+        <v>1.1684232182386179E-4</v>
+      </c>
+      <c r="P6" s="4">
+        <v>9.0555319806772424E-4</v>
+      </c>
+      <c r="S6" s="2">
+        <f>S5+1</f>
+        <v>2</v>
+      </c>
+      <c r="T6" s="4">
+        <v>1.0891381202107789E-4</v>
+      </c>
+      <c r="U6" s="4">
+        <v>7.7944262169602082E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f t="shared" ref="D7:D54" si="0">D6+1</f>
         <v>3</v>
       </c>
       <c r="E7" s="4">
-        <v>1.3064811918610399E-4</v>
+        <v>1.1729558873792271E-4</v>
       </c>
       <c r="F7" s="4">
-        <v>6.1581285621312588E-4</v>
+        <v>6.479797320458633E-4</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" ref="I7:I54" si="1">I6+1</f>
         <v>3</v>
       </c>
-      <c r="J7" s="4">
-        <v>1.0154041121546049E-4</v>
-      </c>
-      <c r="K7" s="4">
-        <v>1.068389897890192E-3</v>
-      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
       <c r="N7" s="2">
         <f t="shared" ref="N7:N54" si="2">N6+1</f>
         <v>3</v>
       </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="O7" s="4">
+        <v>1.3064811918610399E-4</v>
+      </c>
+      <c r="P7" s="4">
+        <v>6.1581285621312588E-4</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" ref="S7:S54" si="3">S6+1</f>
+        <v>3</v>
+      </c>
+      <c r="T7" s="4">
+        <v>1.0154041121546049E-4</v>
+      </c>
+      <c r="U7" s="4">
+        <v>1.068389897890192E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E8" s="4">
+        <v>1.0889641202775369E-4</v>
+      </c>
+      <c r="F8" s="4">
+        <v>9.2767564656161987E-4</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="N8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O8" s="4">
         <v>1.2907266383490931E-4</v>
       </c>
-      <c r="F8" s="4">
+      <c r="P8" s="4">
         <v>8.2228677010219174E-4</v>
       </c>
-      <c r="I8" s="2">
-        <f t="shared" si="1"/>
+      <c r="S8" s="2">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="J8" s="4">
+      <c r="T8" s="4">
         <v>1.118512864312136E-4</v>
       </c>
-      <c r="K8" s="4">
+      <c r="U8" s="4">
         <v>9.3446588667570572E-4</v>
       </c>
-      <c r="N8" s="2">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E9" s="4">
+        <v>1.073067698088286E-4</v>
+      </c>
+      <c r="F9" s="4">
+        <v>9.4970750039003219E-4</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O9" s="4">
         <v>1.196053616554614E-4</v>
       </c>
-      <c r="F9" s="4">
+      <c r="P9" s="4">
         <v>1.131388841680097E-3</v>
       </c>
-      <c r="I9" s="2">
-        <f t="shared" si="1"/>
+      <c r="S9" s="2">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="J9" s="4">
+      <c r="T9" s="4">
         <v>1.1888193294917651E-4</v>
       </c>
-      <c r="K9" s="4">
+      <c r="U9" s="4">
         <v>7.1262290278773692E-4</v>
       </c>
-      <c r="N9" s="2">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E10" s="4">
+        <v>1.2516013817946689E-4</v>
+      </c>
+      <c r="F10" s="4">
+        <v>6.5224743197524898E-4</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O10" s="4">
         <v>1.150768396915385E-4</v>
       </c>
-      <c r="F10" s="4">
+      <c r="P10" s="4">
         <v>8.7877762403024379E-4</v>
       </c>
-      <c r="I10" s="2">
-        <f t="shared" si="1"/>
+      <c r="S10" s="2">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="J10" s="4">
+      <c r="T10" s="4">
         <v>1.103963584647762E-4</v>
       </c>
-      <c r="K10" s="4">
+      <c r="U10" s="4">
         <v>7.8850298554907611E-4</v>
       </c>
-      <c r="N10" s="2">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E11" s="4">
+        <v>1.0821645831922731E-4</v>
+      </c>
+      <c r="F11" s="4">
+        <v>8.4132520959247464E-4</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O11" s="4">
         <v>1.3179345133859961E-4</v>
       </c>
-      <c r="F11" s="4">
+      <c r="P11" s="4">
         <v>8.1214201809106225E-4</v>
       </c>
-      <c r="I11" s="2">
-        <f t="shared" si="1"/>
+      <c r="S11" s="2">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="J11" s="4">
+      <c r="T11" s="4">
         <v>1.170134769518971E-4</v>
       </c>
-      <c r="K11" s="4">
+      <c r="U11" s="4">
         <v>8.2365794256866374E-4</v>
       </c>
-      <c r="N11" s="2">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E12" s="4">
+        <v>1.158497078907479E-4</v>
+      </c>
+      <c r="F12" s="4">
+        <v>7.7206270219347969E-4</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O12" s="4">
         <v>1.27837345502081E-4</v>
       </c>
-      <c r="F12" s="4">
+      <c r="P12" s="4">
         <v>6.5823873704807818E-4</v>
       </c>
-      <c r="I12" s="2">
-        <f t="shared" si="1"/>
+      <c r="S12" s="2">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="J12" s="4">
+      <c r="T12" s="4">
         <v>1.1700085887599451E-4</v>
       </c>
-      <c r="K12" s="4">
+      <c r="U12" s="4">
         <v>8.1303807976297637E-4</v>
       </c>
-      <c r="N12" s="2">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E13" s="4">
+        <v>1.2856290334107149E-4</v>
+      </c>
+      <c r="F13" s="4">
+        <v>4.4797292038909538E-4</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O13" s="4">
         <v>1.3510054044324821E-4</v>
       </c>
-      <c r="F13" s="4">
+      <c r="P13" s="4">
         <v>7.9729353656454911E-4</v>
       </c>
-      <c r="I13" s="2">
-        <f t="shared" si="1"/>
+      <c r="S13" s="2">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="J13" s="4">
+      <c r="T13" s="4">
         <v>1.074416458598002E-4</v>
       </c>
-      <c r="K13" s="4">
+      <c r="U13" s="4">
         <v>8.6743831492659652E-4</v>
       </c>
-      <c r="N13" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E14" s="4">
+        <v>1.130265704787998E-4</v>
+      </c>
+      <c r="F14" s="4">
+        <v>8.671009752670146E-4</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O14" s="4">
         <v>1.2781710482353241E-4</v>
       </c>
-      <c r="F14" s="4">
+      <c r="P14" s="4">
         <v>8.6198401991352677E-4</v>
       </c>
-      <c r="I14" s="2">
-        <f t="shared" si="1"/>
+      <c r="S14" s="2">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="J14" s="4">
+      <c r="T14" s="4">
         <v>1.09577897553583E-4</v>
       </c>
-      <c r="K14" s="4">
+      <c r="U14" s="4">
         <v>7.0802050484675551E-4</v>
       </c>
-      <c r="N14" s="2">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E15" s="4">
+        <v>1.0882650668778401E-4</v>
+      </c>
+      <c r="F15" s="4">
+        <v>7.9354509082349292E-4</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O15" s="4">
         <v>1.2443272577550871E-4</v>
       </c>
-      <c r="F15" s="4">
+      <c r="P15" s="4">
         <v>9.1678116028961565E-4</v>
       </c>
-      <c r="I15" s="2">
-        <f t="shared" si="1"/>
+      <c r="S15" s="2">
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="J15" s="4">
+      <c r="T15" s="4">
         <v>1.1146566473363199E-4</v>
       </c>
-      <c r="K15" s="4">
+      <c r="U15" s="4">
         <v>8.9522427310277511E-4</v>
       </c>
-      <c r="N15" s="2">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-    </row>
-    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E16" s="4">
+        <v>1.204279510330717E-4</v>
+      </c>
+      <c r="F16" s="4">
+        <v>5.7749226309721131E-4</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O16" s="4">
         <v>1.213836928698053E-4</v>
       </c>
-      <c r="F16" s="4">
+      <c r="P16" s="4">
         <v>7.4028997501118885E-4</v>
       </c>
-      <c r="I16" s="2">
-        <f t="shared" si="1"/>
+      <c r="S16" s="2">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="J16" s="4">
+      <c r="T16" s="4">
         <v>1.2881160144035639E-4</v>
       </c>
-      <c r="K16" s="4">
+      <c r="U16" s="4">
         <v>6.0547887566405408E-4</v>
       </c>
-      <c r="N16" s="2">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-    </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="E17" s="4">
+        <v>1.17734960878961E-4</v>
+      </c>
+      <c r="F17" s="4">
+        <v>5.1390732170600501E-4</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O17" s="4">
         <v>1.331033592814548E-4</v>
       </c>
-      <c r="F17" s="4">
+      <c r="P17" s="4">
         <v>7.1142868330732127E-4</v>
       </c>
-      <c r="I17" s="2">
-        <f t="shared" si="1"/>
+      <c r="S17" s="2">
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="J17" s="4">
+      <c r="T17" s="4">
         <v>1.160116806879669E-4</v>
       </c>
-      <c r="K17" s="4">
+      <c r="U17" s="4">
         <v>7.8686201298070033E-4</v>
       </c>
-      <c r="N17" s="2">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="E18" s="4">
+        <v>1.1526672796071879E-4</v>
+      </c>
+      <c r="F18" s="4">
+        <v>7.15273948160038E-4</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O18" s="4">
         <v>1.2588106341208461E-4</v>
       </c>
-      <c r="F18" s="4">
+      <c r="P18" s="4">
         <v>9.6648374952556398E-4</v>
       </c>
-      <c r="I18" s="2">
-        <f t="shared" si="1"/>
+      <c r="S18" s="2">
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="J18" s="4">
+      <c r="T18" s="4">
         <v>1.151920989721826E-4</v>
       </c>
-      <c r="K18" s="4">
+      <c r="U18" s="4">
         <v>6.7529202615455408E-4</v>
       </c>
-      <c r="N18" s="2">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-    </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E19" s="4">
+        <v>1.0285955724842201E-4</v>
+      </c>
+      <c r="F19" s="4">
+        <v>9.1322684660520136E-4</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O19" s="4">
         <v>1.314733622636012E-4</v>
       </c>
-      <c r="F19" s="4">
+      <c r="P19" s="4">
         <v>6.3127001127431099E-4</v>
       </c>
-      <c r="I19" s="2">
-        <f t="shared" si="1"/>
+      <c r="S19" s="2">
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="J19" s="4">
+      <c r="T19" s="4">
         <v>1.113182466093625E-4</v>
       </c>
-      <c r="K19" s="4">
+      <c r="U19" s="4">
         <v>6.4647392807658949E-4</v>
       </c>
-      <c r="N19" s="2">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="E20" s="4">
+        <v>1.135952465256039E-4</v>
+      </c>
+      <c r="F20" s="4">
+        <v>7.3711005721822248E-4</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O20" s="4">
         <v>1.257135650161644E-4</v>
       </c>
-      <c r="F20" s="4">
+      <c r="P20" s="4">
         <v>8.4526032248125754E-4</v>
       </c>
-      <c r="I20" s="2">
-        <f t="shared" si="1"/>
+      <c r="S20" s="2">
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="J20" s="4">
+      <c r="T20" s="4">
         <v>1.0889015129475541E-4</v>
       </c>
-      <c r="K20" s="4">
+      <c r="U20" s="4">
         <v>8.0732353339916466E-4</v>
       </c>
-      <c r="N20" s="2">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-    </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E21" s="4">
+        <v>1.153046406766596E-4</v>
+      </c>
+      <c r="F21" s="4">
+        <v>8.1056330221420878E-4</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O21" s="4">
         <v>1.2205393305489601E-4</v>
       </c>
-      <c r="F21" s="4">
+      <c r="P21" s="4">
         <v>1.1109788447526961E-3</v>
       </c>
-      <c r="I21" s="2">
-        <f t="shared" si="1"/>
+      <c r="S21" s="2">
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="J21" s="4">
+      <c r="T21" s="4">
         <v>1.101115699044487E-4</v>
       </c>
-      <c r="K21" s="4">
+      <c r="U21" s="4">
         <v>9.2270492758206736E-4</v>
       </c>
-      <c r="N21" s="2">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-    </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="E22" s="4">
+        <v>1.160845186994199E-4</v>
+      </c>
+      <c r="F22" s="4">
+        <v>8.1941446101934702E-4</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O22" s="4">
         <v>1.1028568841265881E-4</v>
       </c>
-      <c r="F22" s="4">
+      <c r="P22" s="4">
         <v>1.1593087544397051E-3</v>
       </c>
-      <c r="I22" s="2">
-        <f t="shared" si="1"/>
+      <c r="S22" s="2">
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="J22" s="4">
+      <c r="T22" s="4">
         <v>1.043096559125857E-4</v>
       </c>
-      <c r="K22" s="4">
+      <c r="U22" s="4">
         <v>9.0528088851319038E-4</v>
       </c>
-      <c r="N22" s="2">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-    </row>
-    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="E23" s="4">
+        <v>1.1213908789831201E-4</v>
+      </c>
+      <c r="F23" s="4">
+        <v>8.0468752423743396E-4</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O23" s="4">
         <v>1.2272213239451231E-4</v>
       </c>
-      <c r="F23" s="4">
+      <c r="P23" s="4">
         <v>6.4025357704196805E-4</v>
       </c>
-      <c r="I23" s="2">
-        <f t="shared" si="1"/>
+      <c r="S23" s="2">
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="J23" s="4">
+      <c r="T23" s="4">
         <v>1.194774964722091E-4</v>
       </c>
-      <c r="K23" s="4">
+      <c r="U23" s="4">
         <v>6.3690862694057492E-4</v>
       </c>
-      <c r="N23" s="2">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-    </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="E24" s="4">
+        <v>1.206209671975293E-4</v>
+      </c>
+      <c r="F24" s="4">
+        <v>6.6895900056177621E-4</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O24" s="4">
         <v>1.3148820591888291E-4</v>
       </c>
-      <c r="F24" s="4">
+      <c r="P24" s="4">
         <v>6.9219512382108289E-4</v>
       </c>
-      <c r="I24" s="2">
-        <f t="shared" si="1"/>
+      <c r="S24" s="2">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J24" s="4">
+      <c r="T24" s="4">
         <v>1.158794379207492E-4</v>
       </c>
-      <c r="K24" s="4">
+      <c r="U24" s="4">
         <v>6.6499789872208391E-4</v>
       </c>
-      <c r="N24" s="2">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="E25" s="4">
+        <v>1.214394264621541E-4</v>
+      </c>
+      <c r="F25" s="4">
+        <v>5.4739906989165839E-4</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O25" s="4">
         <v>1.172949587198428E-4</v>
       </c>
-      <c r="F25" s="4">
+      <c r="P25" s="4">
         <v>1.011404424568403E-3</v>
       </c>
-      <c r="I25" s="2">
-        <f t="shared" si="1"/>
+      <c r="S25" s="2">
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="J25" s="4">
+      <c r="T25" s="4">
         <v>1.2006704000425851E-4</v>
       </c>
-      <c r="K25" s="4">
+      <c r="U25" s="4">
         <v>8.2281318734743242E-4</v>
       </c>
-      <c r="N25" s="2">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-    </row>
-    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E26" s="4">
+        <v>1.0770107103449111E-4</v>
+      </c>
+      <c r="F26" s="4">
+        <v>7.7942928085939259E-4</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O26" s="4">
         <v>1.2448820086593781E-4</v>
       </c>
-      <c r="F26" s="4">
+      <c r="P26" s="4">
         <v>6.8853616420052764E-4</v>
       </c>
-      <c r="I26" s="2">
-        <f t="shared" si="1"/>
+      <c r="S26" s="2">
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="J26" s="4">
+      <c r="T26" s="4">
         <v>1.115945781844151E-4</v>
       </c>
-      <c r="K26" s="4">
+      <c r="U26" s="4">
         <v>9.1529136256964373E-4</v>
       </c>
-      <c r="N26" s="2">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-    </row>
-    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="E27" s="4">
+        <v>1.187778729232961E-4</v>
+      </c>
+      <c r="F27" s="4">
+        <v>6.7357580858335754E-4</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O27" s="4">
         <v>1.2257170547112881E-4</v>
       </c>
-      <c r="F27" s="4">
+      <c r="P27" s="4">
         <v>8.4712087769224498E-4</v>
       </c>
-      <c r="I27" s="2">
-        <f t="shared" si="1"/>
+      <c r="S27" s="2">
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="J27" s="4">
+      <c r="T27" s="4">
         <v>1.129101404089035E-4</v>
       </c>
-      <c r="K27" s="4">
+      <c r="U27" s="4">
         <v>8.6871692800225757E-4</v>
       </c>
-      <c r="N27" s="2">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-    </row>
-    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="E28" s="4">
+        <v>1.177453520892058E-4</v>
+      </c>
+      <c r="F28" s="4">
+        <v>7.9252047797919941E-4</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O28" s="4">
         <v>1.1912805621076321E-4</v>
       </c>
-      <c r="F28" s="4">
+      <c r="P28" s="4">
         <v>9.2631664213075119E-4</v>
       </c>
-      <c r="I28" s="2">
-        <f t="shared" si="1"/>
+      <c r="S28" s="2">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="J28" s="4">
+      <c r="T28" s="4">
         <v>1.032695086839765E-4</v>
       </c>
-      <c r="K28" s="4">
+      <c r="U28" s="4">
         <v>9.3603048008748921E-4</v>
       </c>
-      <c r="N28" s="2">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-    </row>
-    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="E29" s="4">
+        <v>1.134355321261554E-4</v>
+      </c>
+      <c r="F29" s="4">
+        <v>9.1479681789973346E-4</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O29" s="4">
         <v>1.2707367681803329E-4</v>
       </c>
-      <c r="F29" s="4">
+      <c r="P29" s="4">
         <v>1.052457409967145E-3</v>
       </c>
-      <c r="I29" s="2">
-        <f t="shared" si="1"/>
+      <c r="S29" s="2">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="J29" s="4">
+      <c r="T29" s="4">
         <v>1.146587046893823E-4</v>
       </c>
-      <c r="K29" s="4">
+      <c r="U29" s="4">
         <v>7.9716837329013134E-4</v>
       </c>
-      <c r="N29" s="2">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-    </row>
-    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="E30" s="4">
+        <v>1.165985112963906E-4</v>
+      </c>
+      <c r="F30" s="4">
+        <v>6.6794889007754489E-4</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O30" s="4">
         <v>1.101209863337655E-4</v>
       </c>
-      <c r="F30" s="4">
+      <c r="P30" s="4">
         <v>1.066169818548743E-3</v>
       </c>
-      <c r="I30" s="2">
-        <f t="shared" si="1"/>
+      <c r="S30" s="2">
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="J30" s="4">
+      <c r="T30" s="4">
         <v>1.02154612558613E-4</v>
       </c>
-      <c r="K30" s="4">
+      <c r="U30" s="4">
         <v>1.3330071317397469E-3</v>
       </c>
-      <c r="N30" s="2">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-    </row>
-    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="E31" s="4">
+        <v>1.113658252099999E-4</v>
+      </c>
+      <c r="F31" s="4">
+        <v>7.4616150919109203E-4</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O31" s="4">
         <v>1.1631411971062931E-4</v>
       </c>
-      <c r="F31" s="4">
+      <c r="P31" s="4">
         <v>8.2252014019582834E-4</v>
       </c>
-      <c r="I31" s="2">
-        <f t="shared" si="1"/>
+      <c r="S31" s="2">
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="J31" s="4">
+      <c r="T31" s="4">
         <v>1.12590788315525E-4</v>
       </c>
-      <c r="K31" s="4">
+      <c r="U31" s="4">
         <v>1.020304846375869E-3</v>
       </c>
-      <c r="N31" s="2">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-    </row>
-    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="E32" s="4">
+        <v>1.0060054878520989E-4</v>
+      </c>
+      <c r="F32" s="4">
+        <v>1.2214971562037331E-3</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O32" s="4">
         <v>1.1691816707344799E-4</v>
       </c>
-      <c r="F32" s="4">
+      <c r="P32" s="4">
         <v>8.4187107257652205E-4</v>
       </c>
-      <c r="I32" s="2">
-        <f t="shared" si="1"/>
+      <c r="S32" s="2">
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="J32" s="4">
+      <c r="T32" s="4">
         <v>1.0841652226814051E-4</v>
       </c>
-      <c r="K32" s="4">
+      <c r="U32" s="4">
         <v>7.8672498185434201E-4</v>
       </c>
-      <c r="N32" s="2">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-    </row>
-    <row r="33" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E33" s="4">
+        <v>1.165481149562201E-4</v>
+      </c>
+      <c r="F33" s="4">
+        <v>7.5161986903080546E-4</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O33" s="4">
         <v>1.186602763214805E-4</v>
       </c>
-      <c r="F33" s="4">
+      <c r="P33" s="4">
         <v>8.439045204805169E-4</v>
       </c>
-      <c r="I33" s="2">
-        <f t="shared" si="1"/>
+      <c r="S33" s="2">
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="J33" s="4">
+      <c r="T33" s="4">
         <v>1.222480652536344E-4</v>
       </c>
-      <c r="K33" s="4">
+      <c r="U33" s="4">
         <v>6.1884673748703611E-4</v>
       </c>
-      <c r="N33" s="2">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-    </row>
-    <row r="34" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="E34" s="4">
+        <v>1.1512045209339931E-4</v>
+      </c>
+      <c r="F34" s="4">
+        <v>8.9693269314264682E-4</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O34" s="4">
         <v>1.1581103370376969E-4</v>
       </c>
-      <c r="F34" s="4">
+      <c r="P34" s="4">
         <v>9.014769022625003E-4</v>
       </c>
-      <c r="I34" s="2">
-        <f t="shared" si="1"/>
+      <c r="S34" s="2">
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="J34" s="4">
+      <c r="T34" s="4">
         <v>1.107273227631967E-4</v>
       </c>
-      <c r="K34" s="4">
+      <c r="U34" s="4">
         <v>7.7734611422439496E-4</v>
       </c>
-      <c r="N34" s="2">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-    </row>
-    <row r="35" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="E35" s="4">
+        <v>1.1048582583653519E-4</v>
+      </c>
+      <c r="F35" s="4">
+        <v>1.0306333577165369E-3</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O35" s="4">
         <v>1.165808712408225E-4</v>
       </c>
-      <c r="F35" s="4">
+      <c r="P35" s="4">
         <v>1.025380525361276E-3</v>
       </c>
-      <c r="I35" s="2">
-        <f t="shared" si="1"/>
+      <c r="S35" s="2">
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="J35" s="4">
+      <c r="T35" s="4">
         <v>1.178908565366489E-4</v>
       </c>
-      <c r="K35" s="4">
+      <c r="U35" s="4">
         <v>6.614372410414719E-4</v>
       </c>
-      <c r="N35" s="2">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-    </row>
-    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="E36" s="4">
+        <v>1.103471243130577E-4</v>
+      </c>
+      <c r="F36" s="4">
+        <v>8.8919975847175146E-4</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O36" s="4">
         <v>1.149138524556614E-4</v>
       </c>
-      <c r="F36" s="4">
+      <c r="P36" s="4">
         <v>1.093108640349606E-3</v>
       </c>
-      <c r="I36" s="2">
-        <f t="shared" si="1"/>
+      <c r="S36" s="2">
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="J36" s="4">
+      <c r="T36" s="4">
         <v>1.061911727931064E-4</v>
       </c>
-      <c r="K36" s="4">
+      <c r="U36" s="4">
         <v>1.0836293647513259E-3</v>
       </c>
-      <c r="N36" s="2">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-    </row>
-    <row r="37" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="E37" s="4">
+        <v>1.1565171979153921E-4</v>
+      </c>
+      <c r="F37" s="4">
+        <v>8.1367508266544548E-4</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O37" s="4">
         <v>1.161721732644664E-4</v>
       </c>
-      <c r="F37" s="4">
+      <c r="P37" s="4">
         <v>9.0313277977909076E-4</v>
       </c>
-      <c r="I37" s="2">
-        <f t="shared" si="1"/>
+      <c r="S37" s="2">
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="J37" s="4">
+      <c r="T37" s="4">
         <v>1.158819714449737E-4</v>
       </c>
-      <c r="K37" s="4">
+      <c r="U37" s="4">
         <v>7.7567000667460467E-4</v>
       </c>
-      <c r="N37" s="2">
-        <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-    </row>
-    <row r="38" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="E38" s="4">
+        <v>9.8882445908653134E-5</v>
+      </c>
+      <c r="F38" s="4">
+        <v>1.044643051338154E-3</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O38" s="4">
         <v>1.2013804201188541E-4</v>
       </c>
-      <c r="F38" s="4">
+      <c r="P38" s="4">
         <v>1.1092219520759631E-3</v>
       </c>
-      <c r="I38" s="2">
-        <f t="shared" si="1"/>
+      <c r="S38" s="2">
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="J38" s="4">
+      <c r="T38" s="4">
         <v>1.214944951135354E-4</v>
       </c>
-      <c r="K38" s="4">
+      <c r="U38" s="4">
         <v>7.1180906644594747E-4</v>
       </c>
-      <c r="N38" s="2">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-    </row>
-    <row r="39" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="E39" s="4">
+        <v>1.195227836321027E-4</v>
+      </c>
+      <c r="F39" s="4">
+        <v>9.2993579443167919E-4</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O39" s="4">
         <v>1.093439754658021E-4</v>
       </c>
-      <c r="F39" s="4">
+      <c r="P39" s="4">
         <v>1.2470696650656221E-3</v>
       </c>
-      <c r="I39" s="2">
-        <f t="shared" si="1"/>
+      <c r="S39" s="2">
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="J39" s="4">
+      <c r="T39" s="4">
         <v>1.100428270499541E-4</v>
       </c>
-      <c r="K39" s="4">
+      <c r="U39" s="4">
         <v>8.365367047279698E-4</v>
       </c>
-      <c r="N39" s="2">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-    </row>
-    <row r="40" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="E40" s="4">
+        <v>1.282639636953376E-4</v>
+      </c>
+      <c r="F40" s="4">
+        <v>5.9584809620541023E-4</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O40" s="4">
         <v>1.3200713218473401E-4</v>
       </c>
-      <c r="F40" s="4">
+      <c r="P40" s="4">
         <v>6.0641842384086134E-4</v>
       </c>
-      <c r="I40" s="2">
-        <f t="shared" si="1"/>
+      <c r="S40" s="2">
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="J40" s="4">
+      <c r="T40" s="4">
         <v>1.1740693895656139E-4</v>
       </c>
-      <c r="K40" s="4">
+      <c r="U40" s="4">
         <v>8.1723582250925149E-4</v>
       </c>
-      <c r="N40" s="2">
-        <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-    </row>
-    <row r="41" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="E41" s="4">
+        <v>1.220206266496699E-4</v>
+      </c>
+      <c r="F41" s="4">
+        <v>6.4254825175603914E-4</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O41" s="4">
         <v>1.243893078757672E-4</v>
       </c>
-      <c r="F41" s="4">
+      <c r="P41" s="4">
         <v>6.4137284660238365E-4</v>
       </c>
-      <c r="I41" s="2">
-        <f t="shared" si="1"/>
+      <c r="S41" s="2">
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="J41" s="4">
+      <c r="T41" s="4">
         <v>1.14375185014424E-4</v>
       </c>
-      <c r="K41" s="4">
+      <c r="U41" s="4">
         <v>8.6023661076441865E-4</v>
       </c>
-      <c r="N41" s="2">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-    </row>
-    <row r="42" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="E42" s="4">
+        <v>1.1077993553596591E-4</v>
+      </c>
+      <c r="F42" s="4">
+        <v>9.1333598165661768E-4</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O42" s="4">
         <v>1.2796915013832901E-4</v>
       </c>
-      <c r="F42" s="4">
+      <c r="P42" s="4">
         <v>7.842184876207509E-4</v>
       </c>
-      <c r="I42" s="2">
-        <f t="shared" si="1"/>
+      <c r="S42" s="2">
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="J42" s="4">
+      <c r="T42" s="4">
         <v>1.159353146501999E-4</v>
       </c>
-      <c r="K42" s="4">
+      <c r="U42" s="4">
         <v>7.2700204670618019E-4</v>
       </c>
-      <c r="N42" s="2">
-        <f t="shared" si="2"/>
-        <v>38</v>
-      </c>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
-    </row>
-    <row r="43" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="E43" s="4">
+        <v>1.056205010701253E-4</v>
+      </c>
+      <c r="F43" s="4">
+        <v>1.21911258611531E-3</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O43" s="4">
         <v>1.26623201515188E-4</v>
       </c>
-      <c r="F43" s="4">
+      <c r="P43" s="4">
         <v>8.4674089676561458E-4</v>
       </c>
-      <c r="I43" s="2">
-        <f t="shared" si="1"/>
+      <c r="S43" s="2">
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="J43" s="4">
+      <c r="T43" s="4">
         <v>1.111612736735101E-4</v>
       </c>
-      <c r="K43" s="4">
+      <c r="U43" s="4">
         <v>7.6137289673025479E-4</v>
       </c>
-      <c r="N43" s="2">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-    </row>
-    <row r="44" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="E44" s="4">
+        <v>1.068333219781326E-4</v>
+      </c>
+      <c r="F44" s="4">
+        <v>9.3976049364988626E-4</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O44" s="4">
         <v>1.14893492568111E-4</v>
       </c>
-      <c r="F44" s="4">
+      <c r="P44" s="4">
         <v>1.1309888794191561E-3</v>
       </c>
-      <c r="I44" s="2">
-        <f t="shared" si="1"/>
+      <c r="S44" s="2">
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="J44" s="4">
+      <c r="T44" s="4">
         <v>1.198889625765995E-4</v>
       </c>
-      <c r="K44" s="4">
+      <c r="U44" s="4">
         <v>6.6171202802765741E-4</v>
       </c>
-      <c r="N44" s="2">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-    </row>
-    <row r="45" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="E45" s="4">
+        <v>1.2035534168523871E-4</v>
+      </c>
+      <c r="F45" s="4">
+        <v>7.0718301864098048E-4</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O45" s="4">
         <v>1.2503425381630269E-4</v>
       </c>
-      <c r="F45" s="4">
+      <c r="P45" s="4">
         <v>8.1257762125139742E-4</v>
       </c>
-      <c r="I45" s="2">
-        <f t="shared" si="1"/>
+      <c r="S45" s="2">
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="J45" s="4">
+      <c r="T45" s="4">
         <v>1.104471776958471E-4</v>
       </c>
-      <c r="K45" s="4">
+      <c r="U45" s="4">
         <v>7.302408854739465E-4</v>
       </c>
-      <c r="N45" s="2">
-        <f t="shared" si="2"/>
-        <v>41</v>
-      </c>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-    </row>
-    <row r="46" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="E46" s="4">
+        <v>1.190085110546975E-4</v>
+      </c>
+      <c r="F46" s="4">
+        <v>5.6326053707049517E-4</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O46" s="4">
         <v>1.0294523615547651E-4</v>
       </c>
-      <c r="F46" s="4">
+      <c r="P46" s="4">
         <v>1.46714595666021E-3</v>
       </c>
-      <c r="I46" s="2">
-        <f t="shared" si="1"/>
+      <c r="S46" s="2">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="J46" s="4">
+      <c r="T46" s="4">
         <v>1.059238435859602E-4</v>
       </c>
-      <c r="K46" s="4">
+      <c r="U46" s="4">
         <v>9.7150380960080705E-4</v>
       </c>
-      <c r="N46" s="2">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-    </row>
-    <row r="47" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="E47" s="4">
+        <v>1.145737984526046E-4</v>
+      </c>
+      <c r="F47" s="4">
+        <v>8.0818621759849534E-4</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O47" s="4">
         <v>1.168407577686567E-4</v>
       </c>
-      <c r="F47" s="4">
+      <c r="P47" s="4">
         <v>8.7897910071153417E-4</v>
       </c>
-      <c r="I47" s="2">
-        <f t="shared" si="1"/>
+      <c r="S47" s="2">
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="J47" s="4">
+      <c r="T47" s="4">
         <v>1.22426004213166E-4</v>
       </c>
-      <c r="K47" s="4">
+      <c r="U47" s="4">
         <v>8.1492842614850898E-4</v>
       </c>
-      <c r="N47" s="2">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-    </row>
-    <row r="48" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="E48" s="4">
+        <v>1.0773346818245979E-4</v>
+      </c>
+      <c r="F48" s="4">
+        <v>9.7311875964503235E-4</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O48" s="4">
         <v>1.221622187447097E-4</v>
       </c>
-      <c r="F48" s="4">
+      <c r="P48" s="4">
         <v>9.8622951537373168E-4</v>
       </c>
-      <c r="I48" s="2">
-        <f t="shared" si="1"/>
+      <c r="S48" s="2">
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="J48" s="4">
+      <c r="T48" s="4">
         <v>1.161235099756959E-4</v>
       </c>
-      <c r="K48" s="4">
+      <c r="U48" s="4">
         <v>7.0573380618306827E-4</v>
       </c>
-      <c r="N48" s="2">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-    </row>
-    <row r="49" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="E49" s="4">
+        <v>1.0986329074547791E-4</v>
+      </c>
+      <c r="F49" s="4">
+        <v>9.45205646369929E-4</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O49" s="4">
         <v>1.187631280360972E-4</v>
       </c>
-      <c r="F49" s="4">
+      <c r="P49" s="4">
         <v>1.057709492025047E-3</v>
       </c>
-      <c r="I49" s="2">
-        <f t="shared" si="1"/>
+      <c r="S49" s="2">
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="J49" s="4">
+      <c r="T49" s="4">
         <v>1.19698277375593E-4</v>
       </c>
-      <c r="K49" s="4">
+      <c r="U49" s="4">
         <v>7.3419598659927438E-4</v>
       </c>
-      <c r="N49" s="2">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-    </row>
-    <row r="50" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="E50" s="4">
+        <v>1.166357855937949E-4</v>
+      </c>
+      <c r="F50" s="4">
+        <v>7.1880030413999684E-4</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O50" s="4">
         <v>1.312275112482064E-4</v>
       </c>
-      <c r="F50" s="4">
+      <c r="P50" s="4">
         <v>8.4211498440781734E-4</v>
       </c>
-      <c r="I50" s="2">
-        <f t="shared" si="1"/>
+      <c r="S50" s="2">
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="J50" s="4">
+      <c r="T50" s="4">
         <v>1.190421091684601E-4</v>
       </c>
-      <c r="K50" s="4">
+      <c r="U50" s="4">
         <v>6.5277229150685634E-4</v>
       </c>
-      <c r="N50" s="2">
-        <f t="shared" si="2"/>
-        <v>46</v>
-      </c>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
-    </row>
-    <row r="51" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="E51" s="4">
+        <v>1.08858134547076E-4</v>
+      </c>
+      <c r="F51" s="4">
+        <v>9.6933942309175721E-4</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O51" s="4">
         <v>1.2471372369474211E-4</v>
       </c>
-      <c r="F51" s="4">
+      <c r="P51" s="4">
         <v>7.4555923734151745E-4</v>
       </c>
-      <c r="I51" s="2">
-        <f t="shared" si="1"/>
+      <c r="S51" s="2">
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="J51" s="4">
+      <c r="T51" s="4">
         <v>1.135124577623107E-4</v>
       </c>
-      <c r="K51" s="4">
+      <c r="U51" s="4">
         <v>1.007523653543452E-3</v>
       </c>
-      <c r="N51" s="2">
-        <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="O51" s="4"/>
-      <c r="P51" s="4"/>
-    </row>
-    <row r="52" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="E52" s="4">
+        <v>1.145990088697952E-4</v>
+      </c>
+      <c r="F52" s="4">
+        <v>7.6348294045123154E-4</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O52" s="4">
         <v>1.113379617603689E-4</v>
       </c>
-      <c r="F52" s="4">
+      <c r="P52" s="4">
         <v>9.5659094739302373E-4</v>
       </c>
-      <c r="I52" s="2">
-        <f t="shared" si="1"/>
+      <c r="S52" s="2">
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="J52" s="4">
+      <c r="T52" s="4">
         <v>1.113164752526531E-4</v>
       </c>
-      <c r="K52" s="4">
+      <c r="U52" s="4">
         <v>8.7143482313756335E-4</v>
       </c>
-      <c r="N52" s="2">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
-    </row>
-    <row r="53" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="E53" s="4">
+        <v>1.1729761060951779E-4</v>
+      </c>
+      <c r="F53" s="4">
+        <v>6.7587944213591089E-4</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O53" s="4">
         <v>1.167654447349066E-4</v>
       </c>
-      <c r="F53" s="4">
+      <c r="P53" s="4">
         <v>9.5188505308882313E-4</v>
       </c>
-      <c r="I53" s="2">
-        <f t="shared" si="1"/>
+      <c r="S53" s="2">
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="J53" s="4">
+      <c r="T53" s="4">
         <v>1.162135403229242E-4</v>
       </c>
-      <c r="K53" s="4">
+      <c r="U53" s="4">
         <v>6.5800478690999616E-4</v>
       </c>
-      <c r="N53" s="2">
-        <f t="shared" si="2"/>
-        <v>49</v>
-      </c>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
-    </row>
-    <row r="54" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="E54" s="4">
+        <v>1.131815744435845E-4</v>
+      </c>
+      <c r="F54" s="4">
+        <v>6.6087692954694215E-4</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="N54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O54" s="4">
         <v>1.279191349390201E-4</v>
       </c>
-      <c r="F54" s="4">
+      <c r="P54" s="4">
         <v>8.439628751452543E-4</v>
       </c>
-      <c r="I54" s="2">
-        <f t="shared" si="1"/>
+      <c r="S54" s="2">
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="J54" s="4">
+      <c r="T54" s="4">
         <v>1.0465679180572701E-4</v>
       </c>
-      <c r="K54" s="4">
+      <c r="U54" s="4">
         <v>1.035666480828549E-3</v>
       </c>
-      <c r="N54" s="2">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
-    </row>
-    <row r="56" spans="4:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E56" s="4">
         <f>AVERAGE(E5:E54)</f>
-        <v>1.2191839352985973E-4</v>
+        <v>1.1417080396261924E-4</v>
       </c>
       <c r="F56" s="4">
         <f>AVERAGE(F5:F54)</f>
-        <v>8.8895756218133957E-4</v>
+        <v>8.0031622215654644E-4</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J56" s="4">
+      <c r="J56" s="4" t="e">
         <f>AVERAGE(J5:J54)</f>
-        <v>1.1334891543117149E-4</v>
-      </c>
-      <c r="K56" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K56" s="4" t="e">
         <f>AVERAGE(K5:K54)</f>
-        <v>8.1685971052536572E-4</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O56" s="4" t="e">
+      <c r="O56" s="4">
         <f>AVERAGE(O5:O54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P56" s="4" t="e">
+        <v>1.2191839352985973E-4</v>
+      </c>
+      <c r="P56" s="4">
         <f>AVERAGE(P5:P54)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="57" spans="4:16" x14ac:dyDescent="0.25">
+        <v>8.8895756218133957E-4</v>
+      </c>
+      <c r="S56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T56" s="4">
+        <f>AVERAGE(T5:T54)</f>
+        <v>1.1334891543117149E-4</v>
+      </c>
+      <c r="U56" s="4">
+        <f>AVERAGE(U5:U54)</f>
+        <v>8.1685971052536572E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E57" s="4">
         <f>_xlfn.STDEV.S(E5:E54)</f>
-        <v>7.1459789974840207E-6</v>
+        <v>6.2523768510112304E-6</v>
       </c>
       <c r="F57" s="4">
         <f>_xlfn.STDEV.S(F5:F54)</f>
-        <v>1.8171701498687141E-4</v>
+        <v>1.6486117721872294E-4</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J57" s="4">
+      <c r="J57" s="4" t="e">
         <f>_xlfn.STDEV.S(J5:J54)</f>
-        <v>5.7543411780092667E-6</v>
-      </c>
-      <c r="K57" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K57" s="4" t="e">
         <f>_xlfn.STDEV.S(K5:K54)</f>
-        <v>1.4234407099589349E-4</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O57" s="4" t="e">
+      <c r="O57" s="4">
         <f>_xlfn.STDEV.S(O5:O54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P57" s="4" t="e">
+        <v>7.1459789974840207E-6</v>
+      </c>
+      <c r="P57" s="4">
         <f>_xlfn.STDEV.S(P5:P54)</f>
-        <v>#DIV/0!</v>
+        <v>1.8171701498687141E-4</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T57" s="4">
+        <f>_xlfn.STDEV.S(T5:T54)</f>
+        <v>5.7543411780092667E-6</v>
+      </c>
+      <c r="U57" s="4">
+        <f>_xlfn.STDEV.S(U5:U54)</f>
+        <v>1.4234407099589349E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
superdataset-20 without cons test on mse
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-3.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-3.xlsx
@@ -2658,8 +2658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2735,8 +2735,12 @@
       <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="J5" s="4">
+        <v>1.260567827915849E-4</v>
+      </c>
+      <c r="K5" s="4">
+        <v>8.8609599328868442E-4</v>
+      </c>
       <c r="N5" s="2">
         <v>1</v>
       </c>
@@ -2771,8 +2775,12 @@
         <f>I5+1</f>
         <v>2</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="J6" s="4">
+        <v>1.299822379837136E-4</v>
+      </c>
+      <c r="K6" s="4">
+        <v>7.3875384176743753E-4</v>
+      </c>
       <c r="N6" s="2">
         <f>N5+1</f>
         <v>2</v>
@@ -2809,8 +2817,12 @@
         <f t="shared" ref="I7:I54" si="1">I6+1</f>
         <v>3</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="J7" s="4">
+        <v>1.3078930621163439E-4</v>
+      </c>
+      <c r="K7" s="4">
+        <v>7.0211228813735042E-4</v>
+      </c>
       <c r="N7" s="2">
         <f t="shared" ref="N7:N54" si="2">N6+1</f>
         <v>3</v>
@@ -2847,8 +2859,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="J8" s="4">
+        <v>1.2278006913106181E-4</v>
+      </c>
+      <c r="K8" s="4">
+        <v>8.5502507398697804E-4</v>
+      </c>
       <c r="N8" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -2885,8 +2901,12 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="J9" s="4">
+        <v>1.218396728429256E-4</v>
+      </c>
+      <c r="K9" s="4">
+        <v>7.9082699613828536E-4</v>
+      </c>
       <c r="N9" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -2923,8 +2943,12 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="J10" s="4">
+        <v>1.3126986203252259E-4</v>
+      </c>
+      <c r="K10" s="4">
+        <v>8.0972213215268975E-4</v>
+      </c>
       <c r="N10" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -2961,8 +2985,12 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="J11" s="4">
+        <v>1.288656729028824E-4</v>
+      </c>
+      <c r="K11" s="4">
+        <v>5.93135595854183E-4</v>
+      </c>
       <c r="N11" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -2999,8 +3027,12 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="J12" s="4">
+        <v>1.153423288888115E-4</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1.0602270190530651E-3</v>
+      </c>
       <c r="N12" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -3037,8 +3069,12 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="J13" s="4">
+        <v>1.206247022007995E-4</v>
+      </c>
+      <c r="K13" s="4">
+        <v>8.7573741621776134E-4</v>
+      </c>
       <c r="N13" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -3075,8 +3111,12 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="J14" s="4">
+        <v>1.205017866461175E-4</v>
+      </c>
+      <c r="K14" s="4">
+        <v>8.0682603068781456E-4</v>
+      </c>
       <c r="N14" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -3113,8 +3153,12 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="J15" s="4">
+        <v>1.28494963953324E-4</v>
+      </c>
+      <c r="K15" s="4">
+        <v>9.1650812249410016E-4</v>
+      </c>
       <c r="N15" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -3151,8 +3195,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="J16" s="4">
+        <v>1.283765813976262E-4</v>
+      </c>
+      <c r="K16" s="4">
+        <v>6.9479160147932354E-4</v>
+      </c>
       <c r="N16" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -3189,8 +3237,12 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="J17" s="4">
+        <v>1.2234398612041269E-4</v>
+      </c>
+      <c r="K17" s="4">
+        <v>7.2183592544594903E-4</v>
+      </c>
       <c r="N17" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -3227,8 +3279,12 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
+      <c r="J18" s="4">
+        <v>1.211528045349201E-4</v>
+      </c>
+      <c r="K18" s="4">
+        <v>1.1120615694756751E-3</v>
+      </c>
       <c r="N18" s="2">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -3265,8 +3321,12 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="J19" s="4">
+        <v>1.2140786483355459E-4</v>
+      </c>
+      <c r="K19" s="4">
+        <v>8.0205079880494472E-4</v>
+      </c>
       <c r="N19" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -3303,8 +3363,12 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="J20" s="4">
+        <v>1.22644555519073E-4</v>
+      </c>
+      <c r="K20" s="4">
+        <v>7.9212406907819646E-4</v>
+      </c>
       <c r="N20" s="2">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -3341,8 +3405,12 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="J21" s="4">
+        <v>1.262607957238438E-4</v>
+      </c>
+      <c r="K21" s="4">
+        <v>8.9358679777960348E-4</v>
+      </c>
       <c r="N21" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -3379,8 +3447,12 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
+      <c r="J22" s="4">
+        <v>1.3167131078080751E-4</v>
+      </c>
+      <c r="K22" s="4">
+        <v>6.997929800938936E-4</v>
+      </c>
       <c r="N22" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -3417,8 +3489,12 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="J23" s="4">
+        <v>1.2734502024996179E-4</v>
+      </c>
+      <c r="K23" s="4">
+        <v>9.2047436841062125E-4</v>
+      </c>
       <c r="N23" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -3455,8 +3531,12 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="J24" s="4">
+        <v>1.264267009847704E-4</v>
+      </c>
+      <c r="K24" s="4">
+        <v>9.4501680502124814E-4</v>
+      </c>
       <c r="N24" s="2">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -3493,8 +3573,12 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="J25" s="4">
+        <v>1.208003758490001E-4</v>
+      </c>
+      <c r="K25" s="4">
+        <v>1.031325876223435E-3</v>
+      </c>
       <c r="N25" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -3531,8 +3615,12 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="J26" s="4">
+        <v>1.3090331775348111E-4</v>
+      </c>
+      <c r="K26" s="4">
+        <v>6.9502658809301348E-4</v>
+      </c>
       <c r="N26" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -3569,8 +3657,12 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="J27" s="4">
+        <v>1.19280870028474E-4</v>
+      </c>
+      <c r="K27" s="4">
+        <v>1.008807098173565E-3</v>
+      </c>
       <c r="N27" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -3607,8 +3699,12 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="J28" s="4">
+        <v>1.2649363776548889E-4</v>
+      </c>
+      <c r="K28" s="4">
+        <v>8.0731188182762395E-4</v>
+      </c>
       <c r="N28" s="2">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -3645,8 +3741,12 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="J29" s="4">
+        <v>1.2267562823929559E-4</v>
+      </c>
+      <c r="K29" s="4">
+        <v>1.1892792231738541E-3</v>
+      </c>
       <c r="N29" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -3683,8 +3783,12 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="J30" s="4">
+        <v>1.12157791070927E-4</v>
+      </c>
+      <c r="K30" s="4">
+        <v>1.1369237280560169E-3</v>
+      </c>
       <c r="N30" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -3721,8 +3825,12 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="J31" s="4">
+        <v>1.3044747241334231E-4</v>
+      </c>
+      <c r="K31" s="4">
+        <v>6.6377997392327534E-4</v>
+      </c>
       <c r="N31" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -3759,8 +3867,12 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="J32" s="4">
+        <v>1.1648007639381439E-4</v>
+      </c>
+      <c r="K32" s="4">
+        <v>1.3587044815867361E-3</v>
+      </c>
       <c r="N32" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -3797,8 +3909,12 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="J33" s="4">
+        <v>1.224841842411452E-4</v>
+      </c>
+      <c r="K33" s="4">
+        <v>1.025608878342284E-3</v>
+      </c>
       <c r="N33" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -3835,8 +3951,12 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="J34" s="4">
+        <v>1.272684550430182E-4</v>
+      </c>
+      <c r="K34" s="4">
+        <v>8.3490364443467241E-4</v>
+      </c>
       <c r="N34" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -3873,8 +3993,12 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
+      <c r="J35" s="4">
+        <v>1.2866750322555479E-4</v>
+      </c>
+      <c r="K35" s="4">
+        <v>7.17364694464678E-4</v>
+      </c>
       <c r="N35" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -3911,8 +4035,12 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
+      <c r="J36" s="4">
+        <v>1.3265605814514141E-4</v>
+      </c>
+      <c r="K36" s="4">
+        <v>6.832482843200726E-4</v>
+      </c>
       <c r="N36" s="2">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -3949,8 +4077,12 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
+      <c r="J37" s="4">
+        <v>1.2991186257052591E-4</v>
+      </c>
+      <c r="K37" s="4">
+        <v>5.6686286723547073E-4</v>
+      </c>
       <c r="N37" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -3987,8 +4119,12 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="J38" s="4">
+        <v>1.220250252783237E-4</v>
+      </c>
+      <c r="K38" s="4">
+        <v>1.0504448754098451E-3</v>
+      </c>
       <c r="N38" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -4025,8 +4161,12 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
+      <c r="J39" s="4">
+        <v>1.2209445548691709E-4</v>
+      </c>
+      <c r="K39" s="4">
+        <v>9.3647869479658238E-4</v>
+      </c>
       <c r="N39" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -4063,8 +4203,12 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
+      <c r="J40" s="4">
+        <v>1.2439359076342851E-4</v>
+      </c>
+      <c r="K40" s="4">
+        <v>9.6545147770985571E-4</v>
+      </c>
       <c r="N40" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -4101,8 +4245,12 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
+      <c r="J41" s="4">
+        <v>1.3096107737999469E-4</v>
+      </c>
+      <c r="K41" s="4">
+        <v>7.6149643306337353E-4</v>
+      </c>
       <c r="N41" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -4139,8 +4287,12 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
+      <c r="J42" s="4">
+        <v>1.2548107266803409E-4</v>
+      </c>
+      <c r="K42" s="4">
+        <v>6.9647754537390427E-4</v>
+      </c>
       <c r="N42" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -4177,8 +4329,12 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+      <c r="J43" s="4">
+        <v>1.2740003126159101E-4</v>
+      </c>
+      <c r="K43" s="4">
+        <v>9.3768594418841024E-4</v>
+      </c>
       <c r="N43" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -4215,8 +4371,12 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
+      <c r="J44" s="4">
+        <v>1.330536623544695E-4</v>
+      </c>
+      <c r="K44" s="4">
+        <v>8.8823340393249823E-4</v>
+      </c>
       <c r="N44" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -4253,8 +4413,12 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
+      <c r="J45" s="4">
+        <v>1.2779039520215721E-4</v>
+      </c>
+      <c r="K45" s="4">
+        <v>6.5136083260081341E-4</v>
+      </c>
       <c r="N45" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -4291,8 +4455,12 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
+      <c r="J46" s="4">
+        <v>1.214142123615475E-4</v>
+      </c>
+      <c r="K46" s="4">
+        <v>9.3091646188093481E-4</v>
+      </c>
       <c r="N46" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -4329,8 +4497,12 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
+      <c r="J47" s="4">
+        <v>1.188251800856886E-4</v>
+      </c>
+      <c r="K47" s="4">
+        <v>9.4420616755005787E-4</v>
+      </c>
       <c r="N47" s="2">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -4367,8 +4539,12 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
+      <c r="J48" s="4">
+        <v>1.3009983434465161E-4</v>
+      </c>
+      <c r="K48" s="4">
+        <v>9.093765616032235E-4</v>
+      </c>
       <c r="N48" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -4405,8 +4581,12 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
+      <c r="J49" s="4">
+        <v>1.2297925447553749E-4</v>
+      </c>
+      <c r="K49" s="4">
+        <v>1.116389392337704E-3</v>
+      </c>
       <c r="N49" s="2">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -4443,8 +4623,12 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
+      <c r="J50" s="4">
+        <v>1.3396589627275889E-4</v>
+      </c>
+      <c r="K50" s="4">
+        <v>8.4146355254407774E-4</v>
+      </c>
       <c r="N50" s="2">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -4481,8 +4665,12 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
+      <c r="J51" s="4">
+        <v>1.2790272706201419E-4</v>
+      </c>
+      <c r="K51" s="4">
+        <v>8.6374972545629402E-4</v>
+      </c>
       <c r="N51" s="2">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -4519,8 +4707,12 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
+      <c r="J52" s="4">
+        <v>1.31336691587187E-4</v>
+      </c>
+      <c r="K52" s="4">
+        <v>6.6900781955597766E-4</v>
+      </c>
       <c r="N52" s="2">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -4557,8 +4749,12 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
+      <c r="J53" s="4">
+        <v>1.2736481373059661E-4</v>
+      </c>
+      <c r="K53" s="4">
+        <v>8.5499840274208528E-4</v>
+      </c>
       <c r="N53" s="2">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -4595,8 +4791,12 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
+      <c r="J54" s="4">
+        <v>1.208351987851741E-4</v>
+      </c>
+      <c r="K54" s="4">
+        <v>9.7873719555829171E-4</v>
+      </c>
       <c r="N54" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -4633,13 +4833,13 @@
       <c r="I56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J56" s="4" t="e">
+      <c r="J56" s="4">
         <f>AVERAGE(J5:J54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K56" s="4" t="e">
+        <v>1.2544654715139256E-4</v>
+      </c>
+      <c r="K56" s="4">
         <f>AVERAGE(K5:K54)</f>
-        <v>#DIV/0!</v>
+        <v>8.6664654263052883E-4</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>2</v>
@@ -4679,13 +4879,13 @@
       <c r="I57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J57" s="4" t="e">
+      <c r="J57" s="4">
         <f>_xlfn.STDEV.S(J5:J54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K57" s="4" t="e">
+        <v>4.9515114189608518E-6</v>
+      </c>
+      <c r="K57" s="4">
         <f>_xlfn.STDEV.S(K5:K54)</f>
-        <v>#DIV/0!</v>
+        <v>1.634608633471507E-4</v>
       </c>
       <c r="N57" s="2" t="s">
         <v>3</v>

</xml_diff>